<commit_message>
IBA assginment 1.3 fixed language
</commit_message>
<xml_diff>
--- a/Introduction_to_Business_Analytics/Assignment/Assignment_1/IBA Assignment (2024-2025) - Data.xlsx
+++ b/Introduction_to_Business_Analytics/Assignment/Assignment_1/IBA Assignment (2024-2025) - Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hektor\Desktop\Kurser\2024-2025\Introduction_to_Business_Analytics\Assignment\Assignment_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hekto\Desktop\Kurser\2024-2025\Introduction_to_Business_Analytics\Assignment\Assignment_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F329185D-A4BC-4F66-A6FA-2D8BA00737CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2288CF40-CC13-4F61-9361-EE0065FC6F0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="8916" tabRatio="893" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="893" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Name and Matriculation Number" sheetId="7" r:id="rId1"/>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="161">
   <si>
     <t>Week</t>
   </si>
@@ -610,9 +610,6 @@
   </si>
   <si>
     <t>Standard Error</t>
-  </si>
-  <si>
-    <t>Conclution:</t>
   </si>
   <si>
     <t>Fail to reject the null hypothesis so thre is not enough evidence to support the claim</t>
@@ -1627,7 +1624,7 @@
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="136">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3"/>
@@ -1841,6 +1838,54 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="57" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="61" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="58" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="57" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="58" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="54" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="55" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="56" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="58" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="58" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="59" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="60" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1895,57 +1940,33 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="58" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="54" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="55" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="56" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="58" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="57" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="58" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="57" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="59" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="60" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="61" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="58" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="46" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="47" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1958,29 +1979,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="46" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="47" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -3086,23 +3086,23 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.88671875" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:3" ht="25.2" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:3" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B6" s="88" t="s">
         <v>111</v>
       </c>
       <c r="C6" s="88"/>
     </row>
-    <row r="7" spans="2:3" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B7" s="33"/>
       <c r="C7" s="33"/>
     </row>
-    <row r="8" spans="2:3" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B8" s="34" t="s">
         <v>109</v>
       </c>
@@ -3110,7 +3110,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B9" s="34" t="s">
         <v>110</v>
       </c>
@@ -3134,28 +3134,28 @@
       <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.6640625" style="6" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.44140625" style="6" customWidth="1"/>
-    <col min="13" max="13" width="4.88671875" style="6" customWidth="1"/>
-    <col min="14" max="14" width="13.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.88671875" style="6"/>
+    <col min="1" max="1" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" style="6" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="6" customWidth="1"/>
+    <col min="13" max="13" width="4.85546875" style="6" customWidth="1"/>
+    <col min="14" max="14" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="23" customFormat="1" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="23" customFormat="1" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>106</v>
       </c>
@@ -3202,7 +3202,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -3255,7 +3255,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
         <v>2</v>
       </c>
@@ -3296,7 +3296,7 @@
         <v>119.25</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
         <v>3</v>
       </c>
@@ -3337,7 +3337,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
         <v>4</v>
       </c>
@@ -3378,7 +3378,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
         <v>5</v>
       </c>
@@ -3419,7 +3419,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
         <v>6</v>
       </c>
@@ -3460,7 +3460,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="14">
         <v>7</v>
       </c>
@@ -3502,7 +3502,7 @@
       </c>
       <c r="M8" s="7"/>
     </row>
-    <row r="9" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
         <v>8</v>
       </c>
@@ -3543,7 +3543,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
         <v>9</v>
       </c>
@@ -3584,7 +3584,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="14">
         <v>10</v>
       </c>
@@ -3625,7 +3625,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="14">
         <v>11</v>
       </c>
@@ -3666,7 +3666,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
         <v>12</v>
       </c>
@@ -3707,7 +3707,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="14">
         <v>13</v>
       </c>
@@ -3748,7 +3748,7 @@
         <v>119.25</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="14">
         <v>14</v>
       </c>
@@ -3789,7 +3789,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
         <v>15</v>
       </c>
@@ -3830,7 +3830,7 @@
         <v>232.20000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="14">
         <v>16</v>
       </c>
@@ -3871,7 +3871,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="14">
         <v>17</v>
       </c>
@@ -3912,7 +3912,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="14">
         <v>18</v>
       </c>
@@ -3953,7 +3953,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="14">
         <v>19</v>
       </c>
@@ -3994,7 +3994,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="14">
         <v>20</v>
       </c>
@@ -4035,7 +4035,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="14">
         <v>21</v>
       </c>
@@ -4076,7 +4076,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="14">
         <v>22</v>
       </c>
@@ -4117,7 +4117,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="14">
         <v>23</v>
       </c>
@@ -4158,7 +4158,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="14">
         <v>24</v>
       </c>
@@ -4199,7 +4199,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="14">
         <v>25</v>
       </c>
@@ -4240,7 +4240,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="14">
         <v>26</v>
       </c>
@@ -4281,7 +4281,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="14">
         <v>27</v>
       </c>
@@ -4322,7 +4322,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="14">
         <v>28</v>
       </c>
@@ -4363,7 +4363,7 @@
         <v>205.65</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="14">
         <v>29</v>
       </c>
@@ -4404,7 +4404,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="14">
         <v>30</v>
       </c>
@@ -4460,128 +4460,128 @@
       <selection activeCell="U23" sqref="U23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="2" customWidth="1"/>
-    <col min="3" max="10" width="9.109375" style="2"/>
+    <col min="3" max="10" width="9.140625" style="2"/>
     <col min="11" max="11" width="9" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="9.109375" style="2"/>
+    <col min="12" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="13" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J14" s="109" t="s">
+    <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J14" s="95" t="s">
         <v>138</v>
       </c>
-      <c r="K14" s="110"/>
-      <c r="L14" s="110"/>
-      <c r="M14" s="110"/>
-      <c r="N14" s="110"/>
-      <c r="O14" s="111"/>
-      <c r="P14" s="119"/>
-      <c r="Q14" s="109" t="s">
+      <c r="K14" s="96"/>
+      <c r="L14" s="96"/>
+      <c r="M14" s="96"/>
+      <c r="N14" s="96"/>
+      <c r="O14" s="97"/>
+      <c r="P14" s="103"/>
+      <c r="Q14" s="95" t="s">
         <v>139</v>
       </c>
-      <c r="R14" s="110"/>
-      <c r="S14" s="111"/>
-    </row>
-    <row r="15" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="92" t="s">
+      <c r="R14" s="96"/>
+      <c r="S14" s="97"/>
+    </row>
+    <row r="15" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="108" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="89" t="s">
+      <c r="B15" s="105" t="s">
         <v>113</v>
       </c>
-      <c r="C15" s="95" t="s">
+      <c r="C15" s="111" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="96"/>
-      <c r="E15" s="97"/>
-      <c r="F15" s="98" t="s">
+      <c r="D15" s="112"/>
+      <c r="E15" s="113"/>
+      <c r="F15" s="114" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="99"/>
-      <c r="H15" s="100"/>
-      <c r="J15" s="112"/>
-      <c r="K15" s="113"/>
-      <c r="L15" s="113"/>
-      <c r="M15" s="113"/>
-      <c r="N15" s="113"/>
-      <c r="O15" s="114"/>
-      <c r="P15" s="120"/>
-      <c r="Q15" s="112"/>
-      <c r="R15" s="113"/>
-      <c r="S15" s="114"/>
-    </row>
-    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="93"/>
-      <c r="B16" s="90"/>
-      <c r="C16" s="101" t="s">
+      <c r="G15" s="115"/>
+      <c r="H15" s="116"/>
+      <c r="J15" s="98"/>
+      <c r="K15" s="99"/>
+      <c r="L15" s="99"/>
+      <c r="M15" s="99"/>
+      <c r="N15" s="99"/>
+      <c r="O15" s="100"/>
+      <c r="P15" s="104"/>
+      <c r="Q15" s="98"/>
+      <c r="R15" s="99"/>
+      <c r="S15" s="100"/>
+    </row>
+    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="109"/>
+      <c r="B16" s="106"/>
+      <c r="C16" s="117" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="103" t="s">
+      <c r="D16" s="119" t="s">
         <v>115</v>
       </c>
-      <c r="E16" s="105" t="s">
+      <c r="E16" s="121" t="s">
         <v>114</v>
       </c>
-      <c r="F16" s="101" t="s">
+      <c r="F16" s="117" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="103" t="s">
+      <c r="G16" s="119" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="105" t="s">
+      <c r="H16" s="121" t="s">
         <v>11</v>
       </c>
-      <c r="J16" s="107" t="s">
+      <c r="J16" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="K16" s="107" t="s">
+      <c r="K16" s="93" t="s">
         <v>115</v>
       </c>
-      <c r="L16" s="107" t="s">
+      <c r="L16" s="93" t="s">
         <v>114</v>
       </c>
-      <c r="M16" s="107" t="s">
+      <c r="M16" s="93" t="s">
         <v>10</v>
       </c>
-      <c r="N16" s="107" t="s">
+      <c r="N16" s="93" t="s">
         <v>9</v>
       </c>
-      <c r="O16" s="107" t="s">
+      <c r="O16" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="P16" s="117"/>
-      <c r="Q16" s="115" t="str">
+      <c r="P16" s="102"/>
+      <c r="Q16" s="101" t="str">
         <f>INDEX(J16:O16, MATCH(Q18, J18:O18, 0))</f>
         <v>α=0.25</v>
       </c>
-      <c r="R16" s="115"/>
-      <c r="S16" s="115"/>
-    </row>
-    <row r="17" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="94"/>
-      <c r="B17" s="91"/>
-      <c r="C17" s="102"/>
-      <c r="D17" s="104"/>
-      <c r="E17" s="106"/>
-      <c r="F17" s="102"/>
-      <c r="G17" s="104"/>
-      <c r="H17" s="106"/>
-      <c r="J17" s="108"/>
-      <c r="K17" s="108"/>
-      <c r="L17" s="108"/>
-      <c r="M17" s="108"/>
-      <c r="N17" s="108"/>
-      <c r="O17" s="108"/>
-      <c r="P17" s="118"/>
-      <c r="Q17" s="116"/>
-      <c r="R17" s="116"/>
-      <c r="S17" s="116"/>
-    </row>
-    <row r="18" spans="1:19" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="R16" s="101"/>
+      <c r="S16" s="101"/>
+    </row>
+    <row r="17" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="110"/>
+      <c r="B17" s="107"/>
+      <c r="C17" s="118"/>
+      <c r="D17" s="120"/>
+      <c r="E17" s="122"/>
+      <c r="F17" s="118"/>
+      <c r="G17" s="120"/>
+      <c r="H17" s="122"/>
+      <c r="J17" s="94"/>
+      <c r="K17" s="94"/>
+      <c r="L17" s="94"/>
+      <c r="M17" s="94"/>
+      <c r="N17" s="94"/>
+      <c r="O17" s="94"/>
+      <c r="P17" s="92"/>
+      <c r="Q17" s="89"/>
+      <c r="R17" s="89"/>
+      <c r="S17" s="89"/>
+    </row>
+    <row r="18" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="48">
         <v>1</v>
       </c>
@@ -4594,39 +4594,39 @@
       <c r="F18" s="37"/>
       <c r="G18" s="40"/>
       <c r="H18" s="41"/>
-      <c r="J18" s="121">
+      <c r="J18" s="90">
         <f>SUMXMY2(B22:B173,C22:C173)/COUNT(C22:C173)</f>
         <v>222.94202302631578</v>
       </c>
-      <c r="K18" s="121">
+      <c r="K18" s="90">
         <f>SUMXMY2(B23:B173,D23:D173)/COUNT(D23:D173)</f>
         <v>215.94172185430466</v>
       </c>
-      <c r="L18" s="121">
+      <c r="L18" s="90">
         <f>SUMXMY2(B24:B173,E24:E173)/COUNT(E24:E173)</f>
         <v>213.54296296296289</v>
       </c>
-      <c r="M18" s="121">
+      <c r="M18" s="90">
         <f>SUMXMY2($B$19:$B$173,F19:F173)/COUNT(F19:F173)</f>
         <v>201.60269314672905</v>
       </c>
-      <c r="N18" s="121">
+      <c r="N18" s="90">
         <f>SUMXMY2($B$19:$B$173,G19:G173)/COUNT(G19:G173)</f>
         <v>233.95925875075537</v>
       </c>
-      <c r="O18" s="121">
+      <c r="O18" s="90">
         <f>SUMXMY2($B$19:$B$173,H19:H173)/COUNT(H19:H173)</f>
         <v>273.77003808044924</v>
       </c>
-      <c r="P18" s="118"/>
-      <c r="Q18" s="116">
+      <c r="P18" s="92"/>
+      <c r="Q18" s="89">
         <f>MIN(J18:O18)</f>
         <v>201.60269314672905</v>
       </c>
-      <c r="R18" s="116"/>
-      <c r="S18" s="116"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R18" s="89"/>
+      <c r="S18" s="89"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="50">
         <v>2</v>
       </c>
@@ -4648,18 +4648,18 @@
         <f>0.75*B18+0.25*B18</f>
         <v>136</v>
       </c>
-      <c r="J19" s="122"/>
-      <c r="K19" s="122"/>
-      <c r="L19" s="122"/>
-      <c r="M19" s="122"/>
-      <c r="N19" s="122"/>
-      <c r="O19" s="122"/>
-      <c r="P19" s="118"/>
-      <c r="Q19" s="116"/>
-      <c r="R19" s="116"/>
-      <c r="S19" s="116"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="J19" s="91"/>
+      <c r="K19" s="91"/>
+      <c r="L19" s="91"/>
+      <c r="M19" s="91"/>
+      <c r="N19" s="91"/>
+      <c r="O19" s="91"/>
+      <c r="P19" s="92"/>
+      <c r="Q19" s="89"/>
+      <c r="R19" s="89"/>
+      <c r="S19" s="89"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="50">
         <v>3</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v>151.75</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="50">
         <v>4</v>
       </c>
@@ -4705,7 +4705,7 @@
         <v>146.6875</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="50">
         <v>5</v>
       </c>
@@ -4731,7 +4731,7 @@
         <v>131.921875</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="50">
         <v>6</v>
       </c>
@@ -4760,7 +4760,7 @@
         <v>146.98046875</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="50">
         <v>7</v>
       </c>
@@ -4792,7 +4792,7 @@
         <v>137.2451171875</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="50">
         <v>8</v>
       </c>
@@ -4824,7 +4824,7 @@
         <v>139.311279296875</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="50">
         <v>9</v>
       </c>
@@ -4856,7 +4856,7 @@
         <v>132.32781982421875</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="50">
         <v>10</v>
       </c>
@@ -4888,7 +4888,7 @@
         <v>142.58195495605469</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="50">
         <v>11</v>
       </c>
@@ -4920,7 +4920,7 @@
         <v>140.64548873901367</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="50">
         <v>12</v>
       </c>
@@ -4952,7 +4952,7 @@
         <v>138.66137218475342</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="50">
         <v>13</v>
       </c>
@@ -4984,7 +4984,7 @@
         <v>140.41534304618835</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="50">
         <v>14</v>
       </c>
@@ -5016,7 +5016,7 @@
         <v>149.10383576154709</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="50">
         <v>15</v>
       </c>
@@ -5048,7 +5048,7 @@
         <v>134.02595894038677</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="50">
         <v>16</v>
       </c>
@@ -5080,7 +5080,7 @@
         <v>148.25648973509669</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="50">
         <v>17</v>
       </c>
@@ -5112,7 +5112,7 @@
         <v>136.06412243377417</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="50">
         <v>18</v>
       </c>
@@ -5144,7 +5144,7 @@
         <v>134.51603060844354</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="50">
         <v>19</v>
       </c>
@@ -5176,7 +5176,7 @@
         <v>130.37900765211089</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="50">
         <v>20</v>
       </c>
@@ -5208,7 +5208,7 @@
         <v>148.09475191302772</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="50">
         <v>21</v>
       </c>
@@ -5240,7 +5240,7 @@
         <v>127.02368797825693</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="50">
         <v>22</v>
       </c>
@@ -5272,7 +5272,7 @@
         <v>120.25592199456423</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="50">
         <v>23</v>
       </c>
@@ -5304,7 +5304,7 @@
         <v>141.81398049864106</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="50">
         <v>24</v>
       </c>
@@ -5336,7 +5336,7 @@
         <v>146.45349512466026</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="50">
         <v>25</v>
       </c>
@@ -5368,7 +5368,7 @@
         <v>125.11337378116507</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="50">
         <v>26</v>
       </c>
@@ -5400,7 +5400,7 @@
         <v>148.27834344529126</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="50">
         <v>27</v>
       </c>
@@ -5432,7 +5432,7 @@
         <v>147.31958586132282</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="50">
         <v>28</v>
       </c>
@@ -5464,7 +5464,7 @@
         <v>153.07989646533071</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="50">
         <v>29</v>
       </c>
@@ -5496,7 +5496,7 @@
         <v>131.26997411633266</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="50">
         <v>30</v>
       </c>
@@ -5528,7 +5528,7 @@
         <v>123.56749352908317</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="50">
         <v>31</v>
       </c>
@@ -5560,7 +5560,7 @@
         <v>149.3918733822708</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="50">
         <v>32</v>
       </c>
@@ -5592,7 +5592,7 @@
         <v>127.34796834556769</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="50">
         <v>33</v>
       </c>
@@ -5624,7 +5624,7 @@
         <v>132.33699208639192</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="50">
         <v>34</v>
       </c>
@@ -5656,7 +5656,7 @@
         <v>140.33424802159797</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="50">
         <v>35</v>
       </c>
@@ -5688,7 +5688,7 @@
         <v>128.0835620053995</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="50">
         <v>36</v>
       </c>
@@ -5720,7 +5720,7 @@
         <v>141.52089050134987</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="50">
         <v>37</v>
       </c>
@@ -5752,7 +5752,7 @@
         <v>132.13022262533747</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="50">
         <v>38</v>
       </c>
@@ -5784,7 +5784,7 @@
         <v>151.53255565633435</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="50">
         <v>39</v>
       </c>
@@ -5816,7 +5816,7 @@
         <v>143.63313891408359</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="50">
         <v>40</v>
       </c>
@@ -5848,7 +5848,7 @@
         <v>146.9082847285209</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="50">
         <v>41</v>
       </c>
@@ -5880,7 +5880,7 @@
         <v>152.22707118213023</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="50">
         <v>42</v>
       </c>
@@ -5912,7 +5912,7 @@
         <v>154.30676779553255</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="50">
         <v>43</v>
       </c>
@@ -5944,7 +5944,7 @@
         <v>138.32669194888314</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="50">
         <v>44</v>
       </c>
@@ -5976,7 +5976,7 @@
         <v>128.33167298722077</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="50">
         <v>45</v>
       </c>
@@ -6008,7 +6008,7 @@
         <v>140.08291824680521</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="50">
         <v>46</v>
       </c>
@@ -6040,7 +6040,7 @@
         <v>126.5207295617013</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="50">
         <v>47</v>
       </c>
@@ -6072,7 +6072,7 @@
         <v>123.88018239042532</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="50">
         <v>48</v>
       </c>
@@ -6104,7 +6104,7 @@
         <v>141.22004559760632</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="50">
         <v>49</v>
       </c>
@@ -6136,7 +6136,7 @@
         <v>154.55501139940156</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="50">
         <v>50</v>
       </c>
@@ -6168,7 +6168,7 @@
         <v>152.63875284985039</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="50">
         <v>51</v>
       </c>
@@ -6200,7 +6200,7 @@
         <v>150.65968821246258</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="50">
         <v>52</v>
       </c>
@@ -6232,7 +6232,7 @@
         <v>126.91492205311565</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="50">
         <v>53</v>
       </c>
@@ -6264,7 +6264,7 @@
         <v>117.97873051327892</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="50">
         <v>54</v>
       </c>
@@ -6296,7 +6296,7 @@
         <v>115.74468262831974</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="50">
         <v>55</v>
       </c>
@@ -6328,7 +6328,7 @@
         <v>148.18617065707994</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="50">
         <v>56</v>
       </c>
@@ -6360,7 +6360,7 @@
         <v>135.29654266426999</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="50">
         <v>57</v>
       </c>
@@ -6392,7 +6392,7 @@
         <v>120.82413566606749</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="50">
         <v>58</v>
       </c>
@@ -6424,7 +6424,7 @@
         <v>125.45603391651687</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="50">
         <v>59</v>
       </c>
@@ -6456,7 +6456,7 @@
         <v>137.11400847912921</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="50">
         <v>60</v>
       </c>
@@ -6488,7 +6488,7 @@
         <v>152.0285021197823</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="50">
         <v>61</v>
       </c>
@@ -6520,7 +6520,7 @@
         <v>126.50712552994557</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="50">
         <v>62</v>
       </c>
@@ -6552,7 +6552,7 @@
         <v>130.6267813824864</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="50">
         <v>63</v>
       </c>
@@ -6584,7 +6584,7 @@
         <v>121.1566953456216</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="50">
         <v>64</v>
       </c>
@@ -6616,7 +6616,7 @@
         <v>131.53917383640541</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="50">
         <v>65</v>
       </c>
@@ -6648,7 +6648,7 @@
         <v>150.63479345910136</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="50">
         <v>66</v>
       </c>
@@ -6680,7 +6680,7 @@
         <v>138.90869836477535</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="50">
         <v>67</v>
       </c>
@@ -6712,7 +6712,7 @@
         <v>144.97717459119383</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="50">
         <v>68</v>
       </c>
@@ -6744,7 +6744,7 @@
         <v>129.99429364779846</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="50">
         <v>69</v>
       </c>
@@ -6776,7 +6776,7 @@
         <v>131.49857341194962</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="50">
         <v>70</v>
       </c>
@@ -6808,7 +6808,7 @@
         <v>119.87464335298741</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="50">
         <v>71</v>
       </c>
@@ -6840,7 +6840,7 @@
         <v>128.21866083824685</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="50">
         <v>72</v>
       </c>
@@ -6872,7 +6872,7 @@
         <v>143.0546652095617</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="50">
         <v>73</v>
       </c>
@@ -6904,7 +6904,7 @@
         <v>143.01366630239042</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="50">
         <v>74</v>
       </c>
@@ -6936,7 +6936,7 @@
         <v>122.00341657559761</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="50">
         <v>75</v>
       </c>
@@ -6968,7 +6968,7 @@
         <v>143.7508541438994</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="50">
         <v>76</v>
       </c>
@@ -7000,7 +7000,7 @@
         <v>152.18771353597486</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="50">
         <v>77</v>
       </c>
@@ -7032,7 +7032,7 @@
         <v>144.5469283839937</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="50">
         <v>78</v>
       </c>
@@ -7064,7 +7064,7 @@
         <v>129.88673209599841</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="50">
         <v>79</v>
       </c>
@@ -7096,7 +7096,7 @@
         <v>131.47168302399962</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="50">
         <v>80</v>
       </c>
@@ -7128,7 +7128,7 @@
         <v>152.1179207559999</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="50">
         <v>81</v>
       </c>
@@ -7160,7 +7160,7 @@
         <v>150.52948018899997</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="50">
         <v>82</v>
       </c>
@@ -7192,7 +7192,7 @@
         <v>141.88237004724999</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="50">
         <v>83</v>
       </c>
@@ -7224,7 +7224,7 @@
         <v>126.9705925118125</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="50">
         <v>84</v>
       </c>
@@ -7256,7 +7256,7 @@
         <v>121.74264812795312</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="50">
         <v>85</v>
       </c>
@@ -7288,7 +7288,7 @@
         <v>119.68566203198827</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="50">
         <v>86</v>
       </c>
@@ -7320,7 +7320,7 @@
         <v>134.92141550799707</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="50">
         <v>87</v>
       </c>
@@ -7352,7 +7352,7 @@
         <v>131.23035387699926</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="50">
         <v>88</v>
       </c>
@@ -7384,7 +7384,7 @@
         <v>124.30758846924982</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="50">
         <v>89</v>
       </c>
@@ -7416,7 +7416,7 @@
         <v>119.57689711731246</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="50">
         <v>90</v>
       </c>
@@ -7448,7 +7448,7 @@
         <v>146.89422427932811</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="50">
         <v>91</v>
       </c>
@@ -7480,7 +7480,7 @@
         <v>140.22355606983203</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="50">
         <v>92</v>
       </c>
@@ -7512,7 +7512,7 @@
         <v>123.55588901745801</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="50">
         <v>93</v>
       </c>
@@ -7544,7 +7544,7 @@
         <v>140.38897225436449</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="50">
         <v>94</v>
       </c>
@@ -7576,7 +7576,7 @@
         <v>138.59724306359112</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="50">
         <v>95</v>
       </c>
@@ -7608,7 +7608,7 @@
         <v>129.14931076589778</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="50">
         <v>96</v>
       </c>
@@ -7640,7 +7640,7 @@
         <v>124.53732769147445</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="50">
         <v>97</v>
       </c>
@@ -7672,7 +7672,7 @@
         <v>121.13433192286861</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="50">
         <v>98</v>
       </c>
@@ -7704,7 +7704,7 @@
         <v>138.28358298071714</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="50">
         <v>99</v>
       </c>
@@ -7736,7 +7736,7 @@
         <v>144.07089574517929</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="50">
         <v>100</v>
       </c>
@@ -7768,7 +7768,7 @@
         <v>144.01772393629483</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="50">
         <v>101</v>
       </c>
@@ -7800,7 +7800,7 @@
         <v>135.00443098407371</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="50">
         <v>102</v>
       </c>
@@ -7832,7 +7832,7 @@
         <v>134.25110774601842</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="50">
         <v>103</v>
       </c>
@@ -7864,7 +7864,7 @@
         <v>125.0627769365046</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="50">
         <v>104</v>
       </c>
@@ -7896,7 +7896,7 @@
         <v>128.76569423412616</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="50">
         <v>105</v>
       </c>
@@ -7928,7 +7928,7 @@
         <v>144.69142355853154</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="50">
         <v>106</v>
       </c>
@@ -7960,7 +7960,7 @@
         <v>153.1728558896329</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="50">
         <v>107</v>
       </c>
@@ -7992,7 +7992,7 @@
         <v>153.79321397240824</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="50">
         <v>108</v>
       </c>
@@ -8024,7 +8024,7 @@
         <v>147.19830349310206</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="50">
         <v>109</v>
       </c>
@@ -8056,7 +8056,7 @@
         <v>153.0495758732755</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="50">
         <v>110</v>
       </c>
@@ -8088,7 +8088,7 @@
         <v>137.26239396831886</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="50">
         <v>111</v>
       </c>
@@ -8120,7 +8120,7 @@
         <v>142.31559849207972</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="50">
         <v>112</v>
       </c>
@@ -8152,7 +8152,7 @@
         <v>133.82889962301994</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="50">
         <v>113</v>
       </c>
@@ -8184,7 +8184,7 @@
         <v>130.20722490575497</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="50">
         <v>114</v>
       </c>
@@ -8216,7 +8216,7 @@
         <v>147.30180622643874</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="50">
         <v>115</v>
       </c>
@@ -8248,7 +8248,7 @@
         <v>136.57545155660969</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="50">
         <v>116</v>
       </c>
@@ -8280,7 +8280,7 @@
         <v>129.39386288915242</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="50">
         <v>117</v>
       </c>
@@ -8312,7 +8312,7 @@
         <v>143.3484657222881</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="50">
         <v>118</v>
       </c>
@@ -8344,7 +8344,7 @@
         <v>146.08711643057202</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="50">
         <v>119</v>
       </c>
@@ -8376,7 +8376,7 @@
         <v>134.021779107643</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="50">
         <v>120</v>
       </c>
@@ -8408,7 +8408,7 @@
         <v>123.50544477691075</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="50">
         <v>121</v>
       </c>
@@ -8440,7 +8440,7 @@
         <v>141.87636119422768</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="50">
         <v>122</v>
       </c>
@@ -8472,7 +8472,7 @@
         <v>136.71909029855692</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="50">
         <v>123</v>
       </c>
@@ -8504,7 +8504,7 @@
         <v>141.42977257463923</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="50">
         <v>124</v>
       </c>
@@ -8536,7 +8536,7 @@
         <v>135.85744314365979</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="50">
         <v>125</v>
       </c>
@@ -8568,7 +8568,7 @@
         <v>146.46436078591495</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="50">
         <v>126</v>
       </c>
@@ -8600,7 +8600,7 @@
         <v>145.36609019647875</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="50">
         <v>127</v>
       </c>
@@ -8632,7 +8632,7 @@
         <v>122.59152254911969</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="50">
         <v>128</v>
       </c>
@@ -8664,7 +8664,7 @@
         <v>149.14788063727991</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="50">
         <v>129</v>
       </c>
@@ -8696,7 +8696,7 @@
         <v>148.28697015931999</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="50">
         <v>130</v>
       </c>
@@ -8728,7 +8728,7 @@
         <v>132.32174253982998</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="50">
         <v>131</v>
       </c>
@@ -8760,7 +8760,7 @@
         <v>138.0804356349575</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="50">
         <v>132</v>
       </c>
@@ -8792,7 +8792,7 @@
         <v>126.02010890873937</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="50">
         <v>133</v>
       </c>
@@ -8824,7 +8824,7 @@
         <v>122.25502722718484</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="50">
         <v>134</v>
       </c>
@@ -8856,7 +8856,7 @@
         <v>133.31375680679622</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="50">
         <v>135</v>
       </c>
@@ -8888,7 +8888,7 @@
         <v>152.57843920169904</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="50">
         <v>136</v>
       </c>
@@ -8920,7 +8920,7 @@
         <v>145.39460980042475</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="50">
         <v>137</v>
       </c>
@@ -8952,7 +8952,7 @@
         <v>124.84865245010619</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="50">
         <v>138</v>
       </c>
@@ -8984,7 +8984,7 @@
         <v>131.71216311252655</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="50">
         <v>139</v>
       </c>
@@ -9016,7 +9016,7 @@
         <v>125.92804077813165</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="50">
         <v>140</v>
       </c>
@@ -9048,7 +9048,7 @@
         <v>128.2320101945329</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="50">
         <v>141</v>
       </c>
@@ -9080,7 +9080,7 @@
         <v>137.80800254863323</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="50">
         <v>142</v>
       </c>
@@ -9112,7 +9112,7 @@
         <v>148.45200063715831</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="50">
         <v>143</v>
       </c>
@@ -9144,7 +9144,7 @@
         <v>150.36300015928958</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="50">
         <v>144</v>
       </c>
@@ -9176,7 +9176,7 @@
         <v>129.09075003982241</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="50">
         <v>145</v>
       </c>
@@ -9208,7 +9208,7 @@
         <v>131.2726875099556</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="50">
         <v>146</v>
       </c>
@@ -9240,7 +9240,7 @@
         <v>122.81817187748891</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="50">
         <v>147</v>
       </c>
@@ -9272,7 +9272,7 @@
         <v>127.45454296937223</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="50">
         <v>148</v>
       </c>
@@ -9304,7 +9304,7 @@
         <v>127.11363574234306</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="50">
         <v>149</v>
       </c>
@@ -9336,7 +9336,7 @@
         <v>144.27840893558576</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="50">
         <v>150</v>
       </c>
@@ -9368,7 +9368,7 @@
         <v>135.81960223389643</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="50">
         <v>151</v>
       </c>
@@ -9400,7 +9400,7 @@
         <v>153.20490055847409</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="50">
         <v>152</v>
       </c>
@@ -9432,7 +9432,7 @@
         <v>135.05122513961851</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="50">
         <v>153</v>
       </c>
@@ -9464,7 +9464,7 @@
         <v>150.76280628490463</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="50">
         <v>154</v>
       </c>
@@ -9496,7 +9496,7 @@
         <v>137.44070157122616</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" s="50">
         <v>155</v>
       </c>
@@ -9528,7 +9528,7 @@
         <v>131.86017539280652</v>
       </c>
     </row>
-    <row r="173" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="52">
         <v>156</v>
       </c>
@@ -9560,7 +9560,7 @@
         <v>123.71504384820163</v>
       </c>
     </row>
-    <row r="174" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="54">
         <v>157</v>
       </c>
@@ -9590,7 +9590,7 @@
         <v>124.6787609620504</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="45"/>
       <c r="B175" s="45"/>
       <c r="C175" s="45"/>
@@ -9600,7 +9600,7 @@
       <c r="G175" s="45"/>
       <c r="H175" s="45"/>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="45"/>
       <c r="B176" s="46"/>
       <c r="C176" s="45"/>
@@ -9610,7 +9610,7 @@
       <c r="G176" s="45"/>
       <c r="H176" s="45"/>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" s="45"/>
       <c r="B177" s="45"/>
       <c r="C177" s="45"/>
@@ -9620,7 +9620,7 @@
       <c r="G177" s="45"/>
       <c r="H177" s="45"/>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" s="47"/>
       <c r="B178" s="47"/>
       <c r="C178" s="47"/>
@@ -9630,7 +9630,7 @@
       <c r="G178" s="47"/>
       <c r="H178" s="47"/>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" s="47"/>
       <c r="B179" s="47"/>
       <c r="C179" s="47"/>
@@ -9640,7 +9640,7 @@
       <c r="G179" s="47"/>
       <c r="H179" s="47"/>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" s="47"/>
       <c r="B180" s="47"/>
       <c r="C180" s="47"/>
@@ -9652,14 +9652,16 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="Q18:S19"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="N18:N19"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="P18:P19"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
     <mergeCell ref="O16:O17"/>
     <mergeCell ref="J14:O15"/>
     <mergeCell ref="Q16:S17"/>
@@ -9671,16 +9673,14 @@
     <mergeCell ref="L16:L17"/>
     <mergeCell ref="M16:M17"/>
     <mergeCell ref="N16:N17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="Q18:S19"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="P18:P19"/>
   </mergeCells>
   <phoneticPr fontId="24" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9691,50 +9691,50 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B4:E30"/>
+  <dimension ref="B4:E28"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="1"/>
-    <col min="2" max="2" width="33.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="47.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="33.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="47.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4"/>
       <c r="C4"/>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5"/>
       <c r="C5"/>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6"/>
       <c r="C6"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7"/>
       <c r="C7"/>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8"/>
       <c r="C8"/>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9"/>
       <c r="C9"/>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
     </row>
-    <row r="11" spans="2:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="123" t="s">
         <v>3</v>
       </c>
@@ -9745,7 +9745,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="123"/>
       <c r="C12" s="86" t="s">
         <v>141</v>
@@ -9754,11 +9754,11 @@
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="36"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>112</v>
       </c>
@@ -9767,10 +9767,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C15" s="36"/>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>4</v>
       </c>
@@ -9784,12 +9784,12 @@
       </c>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C17" s="36"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>5</v>
       </c>
@@ -9803,16 +9803,18 @@
       </c>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C19" s="36"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="35"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C20" s="136" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
         <v>142</v>
       </c>
@@ -9820,7 +9822,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
         <v>143</v>
       </c>
@@ -9828,7 +9830,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
         <v>144</v>
       </c>
@@ -9836,7 +9838,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
         <v>145</v>
       </c>
@@ -9844,7 +9846,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>148</v>
       </c>
@@ -9852,21 +9854,13 @@
         <v>88.5</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
         <v>149</v>
       </c>
       <c r="C28" s="1">
         <f>C23/SQRT(C26)</f>
         <v>1.5</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C30" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -9884,34 +9878,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:XFD1048575"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="71" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="71" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="A17" sqref="A17:B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="12.44140625" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" customWidth="1"/>
-    <col min="7" max="7" width="37.109375" customWidth="1"/>
-    <col min="8" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.44140625" customWidth="1"/>
-    <col min="11" max="11" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="37.140625" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" customWidth="1"/>
+    <col min="11" max="11" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G2" s="132"/>
-      <c r="H2" s="132"/>
+    <row r="2" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="G2" s="128"/>
+      <c r="H2" s="128"/>
       <c r="K2" s="59"/>
       <c r="L2" s="59"/>
     </row>
-    <row r="3" spans="1:12" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="134" t="s">
+    <row r="3" spans="1:12" ht="47.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="130" t="s">
         <v>116</v>
       </c>
-      <c r="B3" s="134"/>
+      <c r="B3" s="130"/>
       <c r="C3" s="60" t="s">
         <v>117</v>
       </c>
@@ -9922,18 +9916,18 @@
         <v>119</v>
       </c>
       <c r="F3" s="58"/>
-      <c r="G3" s="133" t="s">
+      <c r="G3" s="129" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="133"/>
+      <c r="H3" s="129"/>
       <c r="I3" s="58"/>
       <c r="J3" s="60"/>
       <c r="K3" s="61" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="135" t="s">
+    <row r="4" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="131" t="s">
         <v>120</v>
       </c>
       <c r="B4" s="81" t="s">
@@ -9945,7 +9939,7 @@
       <c r="D4" s="67">
         <v>4000</v>
       </c>
-      <c r="E4" s="130">
+      <c r="E4" s="126">
         <v>10000</v>
       </c>
       <c r="F4" s="58"/>
@@ -9959,8 +9953,8 @@
       </c>
       <c r="K4" s="62"/>
     </row>
-    <row r="5" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="129"/>
+    <row r="5" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="125"/>
       <c r="B5" s="68" t="s">
         <v>133</v>
       </c>
@@ -9970,7 +9964,7 @@
       <c r="D5" s="70">
         <v>1500</v>
       </c>
-      <c r="E5" s="131"/>
+      <c r="E5" s="127"/>
       <c r="F5" s="58"/>
       <c r="G5" s="56" t="s">
         <v>125</v>
@@ -9980,8 +9974,8 @@
       <c r="J5" s="58"/>
       <c r="K5" s="58"/>
     </row>
-    <row r="6" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="128" t="s">
+    <row r="6" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="124" t="s">
         <v>121</v>
       </c>
       <c r="B6" s="65" t="s">
@@ -9993,7 +9987,7 @@
       <c r="D6" s="67">
         <v>2000</v>
       </c>
-      <c r="E6" s="130">
+      <c r="E6" s="126">
         <v>3000</v>
       </c>
       <c r="F6" s="58"/>
@@ -10005,8 +9999,8 @@
       <c r="J6" s="58"/>
       <c r="K6" s="58"/>
     </row>
-    <row r="7" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="129"/>
+    <row r="7" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="125"/>
       <c r="B7" s="82" t="s">
         <v>132</v>
       </c>
@@ -10016,7 +10010,7 @@
       <c r="D7" s="70">
         <v>1200</v>
       </c>
-      <c r="E7" s="131"/>
+      <c r="E7" s="127"/>
       <c r="F7" s="58"/>
       <c r="G7" s="56" t="s">
         <v>126</v>
@@ -10026,8 +10020,8 @@
       <c r="J7" s="58"/>
       <c r="K7" s="58"/>
     </row>
-    <row r="8" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="128" t="s">
+    <row r="8" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="124" t="s">
         <v>122</v>
       </c>
       <c r="B8" s="65" t="s">
@@ -10039,7 +10033,7 @@
       <c r="D8" s="66">
         <v>1000</v>
       </c>
-      <c r="E8" s="130">
+      <c r="E8" s="126">
         <v>1000</v>
       </c>
       <c r="F8" s="58"/>
@@ -10051,8 +10045,8 @@
       <c r="J8" s="58"/>
       <c r="K8" s="58"/>
     </row>
-    <row r="9" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="129"/>
+    <row r="9" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="125"/>
       <c r="B9" s="82" t="s">
         <v>135</v>
       </c>
@@ -10062,7 +10056,7 @@
       <c r="D9" s="75">
         <v>800</v>
       </c>
-      <c r="E9" s="131"/>
+      <c r="E9" s="127"/>
       <c r="F9" s="58"/>
       <c r="G9" s="57" t="s">
         <v>128</v>
@@ -10072,354 +10066,354 @@
       <c r="J9" s="58"/>
       <c r="K9" s="58"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="124" t="s">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="132" t="s">
+        <v>151</v>
+      </c>
+      <c r="B12" s="133"/>
+      <c r="C12" s="133"/>
+      <c r="D12" s="133"/>
+      <c r="E12" s="133"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="133"/>
+      <c r="B13" s="133"/>
+      <c r="C13" s="133"/>
+      <c r="D13" s="133"/>
+      <c r="E13" s="133"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="134" t="s">
+        <v>160</v>
+      </c>
+      <c r="B14" s="135"/>
+      <c r="C14" s="135"/>
+      <c r="D14" s="135"/>
+      <c r="E14" s="135"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="135"/>
+      <c r="B15" s="135"/>
+      <c r="C15" s="135"/>
+      <c r="D15" s="135"/>
+      <c r="E15" s="135"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="135"/>
+      <c r="B16" s="135"/>
+      <c r="C16" s="135"/>
+      <c r="D16" s="135"/>
+      <c r="E16" s="135"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="132" t="s">
         <v>152</v>
       </c>
-      <c r="B12" s="125"/>
-      <c r="C12" s="125"/>
-      <c r="D12" s="125"/>
-      <c r="E12" s="125"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="125"/>
-      <c r="B13" s="125"/>
-      <c r="C13" s="125"/>
-      <c r="D13" s="125"/>
-      <c r="E13" s="125"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="126" t="s">
-        <v>161</v>
-      </c>
-      <c r="B14" s="127"/>
-      <c r="C14" s="127"/>
-      <c r="D14" s="127"/>
-      <c r="E14" s="127"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="127"/>
-      <c r="B15" s="127"/>
-      <c r="C15" s="127"/>
-      <c r="D15" s="127"/>
-      <c r="E15" s="127"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="127"/>
-      <c r="B16" s="127"/>
-      <c r="C16" s="127"/>
-      <c r="D16" s="127"/>
-      <c r="E16" s="127"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="124" t="s">
+      <c r="B17" s="133"/>
+      <c r="C17" s="133"/>
+      <c r="D17" s="133"/>
+      <c r="E17" s="133"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="133"/>
+      <c r="B18" s="133"/>
+      <c r="C18" s="133"/>
+      <c r="D18" s="133"/>
+      <c r="E18" s="133"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="132" t="s">
+        <v>156</v>
+      </c>
+      <c r="B19" s="133"/>
+      <c r="C19" s="133"/>
+      <c r="D19" s="133"/>
+      <c r="E19" s="133"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="133"/>
+      <c r="B20" s="133"/>
+      <c r="C20" s="133"/>
+      <c r="D20" s="133"/>
+      <c r="E20" s="133"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="133"/>
+      <c r="B21" s="133"/>
+      <c r="C21" s="133"/>
+      <c r="D21" s="133"/>
+      <c r="E21" s="133"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="132" t="s">
         <v>153</v>
       </c>
-      <c r="B17" s="125"/>
-      <c r="C17" s="125"/>
-      <c r="D17" s="125"/>
-      <c r="E17" s="125"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="125"/>
-      <c r="B18" s="125"/>
-      <c r="C18" s="125"/>
-      <c r="D18" s="125"/>
-      <c r="E18" s="125"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="124" t="s">
+      <c r="B22" s="133"/>
+      <c r="C22" s="133"/>
+      <c r="D22" s="133"/>
+      <c r="E22" s="133"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="133"/>
+      <c r="B23" s="133"/>
+      <c r="C23" s="133"/>
+      <c r="D23" s="133"/>
+      <c r="E23" s="133"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="132" t="s">
         <v>157</v>
       </c>
-      <c r="B19" s="125"/>
-      <c r="C19" s="125"/>
-      <c r="D19" s="125"/>
-      <c r="E19" s="125"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="125"/>
-      <c r="B20" s="125"/>
-      <c r="C20" s="125"/>
-      <c r="D20" s="125"/>
-      <c r="E20" s="125"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="125"/>
-      <c r="B21" s="125"/>
-      <c r="C21" s="125"/>
-      <c r="D21" s="125"/>
-      <c r="E21" s="125"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="124" t="s">
+      <c r="B24" s="133"/>
+      <c r="C24" s="133"/>
+      <c r="D24" s="133"/>
+      <c r="E24" s="133"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="133"/>
+      <c r="B25" s="133"/>
+      <c r="C25" s="133"/>
+      <c r="D25" s="133"/>
+      <c r="E25" s="133"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="133"/>
+      <c r="B26" s="133"/>
+      <c r="C26" s="133"/>
+      <c r="D26" s="133"/>
+      <c r="E26" s="133"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="132" t="s">
         <v>154</v>
       </c>
-      <c r="B22" s="125"/>
-      <c r="C22" s="125"/>
-      <c r="D22" s="125"/>
-      <c r="E22" s="125"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="125"/>
-      <c r="B23" s="125"/>
-      <c r="C23" s="125"/>
-      <c r="D23" s="125"/>
-      <c r="E23" s="125"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="124" t="s">
+      <c r="B27" s="133"/>
+      <c r="C27" s="133"/>
+      <c r="D27" s="133"/>
+      <c r="E27" s="133"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="133"/>
+      <c r="B28" s="133"/>
+      <c r="C28" s="133"/>
+      <c r="D28" s="133"/>
+      <c r="E28" s="133"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="132" t="s">
         <v>158</v>
       </c>
-      <c r="B24" s="125"/>
-      <c r="C24" s="125"/>
-      <c r="D24" s="125"/>
-      <c r="E24" s="125"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="125"/>
-      <c r="B25" s="125"/>
-      <c r="C25" s="125"/>
-      <c r="D25" s="125"/>
-      <c r="E25" s="125"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="125"/>
-      <c r="B26" s="125"/>
-      <c r="C26" s="125"/>
-      <c r="D26" s="125"/>
-      <c r="E26" s="125"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="124" t="s">
+      <c r="B29" s="133"/>
+      <c r="C29" s="133"/>
+      <c r="D29" s="133"/>
+      <c r="E29" s="133"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="133"/>
+      <c r="B30" s="133"/>
+      <c r="C30" s="133"/>
+      <c r="D30" s="133"/>
+      <c r="E30" s="133"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="133"/>
+      <c r="B31" s="133"/>
+      <c r="C31" s="133"/>
+      <c r="D31" s="133"/>
+      <c r="E31" s="133"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="132" t="s">
         <v>155</v>
       </c>
-      <c r="B27" s="125"/>
-      <c r="C27" s="125"/>
-      <c r="D27" s="125"/>
-      <c r="E27" s="125"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="125"/>
-      <c r="B28" s="125"/>
-      <c r="C28" s="125"/>
-      <c r="D28" s="125"/>
-      <c r="E28" s="125"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="124" t="s">
+      <c r="B32" s="133"/>
+      <c r="C32" s="133"/>
+      <c r="D32" s="133"/>
+      <c r="E32" s="133"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="133"/>
+      <c r="B33" s="133"/>
+      <c r="C33" s="133"/>
+      <c r="D33" s="133"/>
+      <c r="E33" s="133"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="132" t="s">
         <v>159</v>
       </c>
-      <c r="B29" s="125"/>
-      <c r="C29" s="125"/>
-      <c r="D29" s="125"/>
-      <c r="E29" s="125"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="125"/>
-      <c r="B30" s="125"/>
-      <c r="C30" s="125"/>
-      <c r="D30" s="125"/>
-      <c r="E30" s="125"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="125"/>
-      <c r="B31" s="125"/>
-      <c r="C31" s="125"/>
-      <c r="D31" s="125"/>
-      <c r="E31" s="125"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="124" t="s">
-        <v>156</v>
-      </c>
-      <c r="B32" s="125"/>
-      <c r="C32" s="125"/>
-      <c r="D32" s="125"/>
-      <c r="E32" s="125"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="125"/>
-      <c r="B33" s="125"/>
-      <c r="C33" s="125"/>
-      <c r="D33" s="125"/>
-      <c r="E33" s="125"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="124" t="s">
-        <v>160</v>
-      </c>
-      <c r="B34" s="125"/>
-      <c r="C34" s="125"/>
-      <c r="D34" s="125"/>
-      <c r="E34" s="125"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="125"/>
-      <c r="B35" s="125"/>
-      <c r="C35" s="125"/>
-      <c r="D35" s="125"/>
-      <c r="E35" s="125"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="125"/>
-      <c r="B36" s="125"/>
-      <c r="C36" s="125"/>
-      <c r="D36" s="125"/>
-      <c r="E36" s="125"/>
-    </row>
-    <row r="37" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1048550" spans="16384:16384" x14ac:dyDescent="0.25">
+      <c r="B34" s="133"/>
+      <c r="C34" s="133"/>
+      <c r="D34" s="133"/>
+      <c r="E34" s="133"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="133"/>
+      <c r="B35" s="133"/>
+      <c r="C35" s="133"/>
+      <c r="D35" s="133"/>
+      <c r="E35" s="133"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="133"/>
+      <c r="B36" s="133"/>
+      <c r="C36" s="133"/>
+      <c r="D36" s="133"/>
+      <c r="E36" s="133"/>
+    </row>
+    <row r="37" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048550" spans="16384:16384" x14ac:dyDescent="0.2">
       <c r="XFD1048550">
         <f>solver_pre</f>
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="1048551" spans="16384:16384" x14ac:dyDescent="0.25">
+    <row r="1048551" spans="16384:16384" x14ac:dyDescent="0.2">
       <c r="XFD1048551">
         <f>solver_scl</f>
         <v>2</v>
       </c>
     </row>
-    <row r="1048552" spans="16384:16384" x14ac:dyDescent="0.25">
+    <row r="1048552" spans="16384:16384" x14ac:dyDescent="0.2">
       <c r="XFD1048552">
         <f>solver_rlx</f>
         <v>2</v>
       </c>
     </row>
-    <row r="1048553" spans="16384:16384" x14ac:dyDescent="0.25">
+    <row r="1048553" spans="16384:16384" x14ac:dyDescent="0.2">
       <c r="XFD1048553">
         <f>solver_tol</f>
         <v>0.01</v>
       </c>
     </row>
-    <row r="1048554" spans="16384:16384" x14ac:dyDescent="0.25">
+    <row r="1048554" spans="16384:16384" x14ac:dyDescent="0.2">
       <c r="XFD1048554">
         <f>solver_cvg</f>
         <v>1E-4</v>
       </c>
     </row>
-    <row r="1048555" spans="16384:16384" x14ac:dyDescent="0.25">
+    <row r="1048555" spans="16384:16384" x14ac:dyDescent="0.2">
       <c r="XFD1048555" t="e" cm="1">
         <f t="array" ref="XFD1048555">AREAS(solver_adj1)</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="1048556" spans="16384:16384" x14ac:dyDescent="0.25">
+    <row r="1048556" spans="16384:16384" x14ac:dyDescent="0.2">
       <c r="XFD1048556">
         <f>solver_ssz</f>
         <v>100</v>
       </c>
     </row>
-    <row r="1048557" spans="16384:16384" x14ac:dyDescent="0.25">
+    <row r="1048557" spans="16384:16384" x14ac:dyDescent="0.2">
       <c r="XFD1048557">
         <f>solver_rsd</f>
         <v>0</v>
       </c>
     </row>
-    <row r="1048558" spans="16384:16384" x14ac:dyDescent="0.25">
+    <row r="1048558" spans="16384:16384" x14ac:dyDescent="0.2">
       <c r="XFD1048558">
         <f>solver_mrt</f>
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="1048559" spans="16384:16384" x14ac:dyDescent="0.25">
+    <row r="1048559" spans="16384:16384" x14ac:dyDescent="0.2">
       <c r="XFD1048559">
         <f>solver_mni</f>
         <v>30</v>
       </c>
     </row>
-    <row r="1048560" spans="16384:16384" x14ac:dyDescent="0.25">
+    <row r="1048560" spans="16384:16384" x14ac:dyDescent="0.2">
       <c r="XFD1048560">
         <f>solver_rbv</f>
         <v>2</v>
       </c>
     </row>
-    <row r="1048561" spans="16384:16384" x14ac:dyDescent="0.25">
+    <row r="1048561" spans="16384:16384" x14ac:dyDescent="0.2">
       <c r="XFD1048561">
         <f>solver_neg</f>
         <v>2</v>
       </c>
     </row>
-    <row r="1048562" spans="16384:16384" x14ac:dyDescent="0.25">
+    <row r="1048562" spans="16384:16384" x14ac:dyDescent="0.2">
       <c r="XFD1048562" t="e" cm="1">
         <f t="array" ref="XFD1048562">solver_ntr</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="1048563" spans="16384:16384" x14ac:dyDescent="0.25">
+    <row r="1048563" spans="16384:16384" x14ac:dyDescent="0.2">
       <c r="XFD1048563" t="e" cm="1">
         <f t="array" ref="XFD1048563">solver_acc</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="1048564" spans="16384:16384" x14ac:dyDescent="0.25">
+    <row r="1048564" spans="16384:16384" x14ac:dyDescent="0.2">
       <c r="XFD1048564" t="e" cm="1">
         <f t="array" ref="XFD1048564">solver_res</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="1048565" spans="16384:16384" x14ac:dyDescent="0.25">
+    <row r="1048565" spans="16384:16384" x14ac:dyDescent="0.2">
       <c r="XFD1048565" t="e" cm="1">
         <f t="array" ref="XFD1048565">solver_ars</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="1048566" spans="16384:16384" x14ac:dyDescent="0.25">
+    <row r="1048566" spans="16384:16384" x14ac:dyDescent="0.2">
       <c r="XFD1048566" t="e" cm="1">
         <f t="array" ref="XFD1048566">solver_sta</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="1048567" spans="16384:16384" x14ac:dyDescent="0.25">
+    <row r="1048567" spans="16384:16384" x14ac:dyDescent="0.2">
       <c r="XFD1048567" t="e" cm="1">
         <f t="array" ref="XFD1048567">solver_met</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="1048568" spans="16384:16384" x14ac:dyDescent="0.25">
+    <row r="1048568" spans="16384:16384" x14ac:dyDescent="0.2">
       <c r="XFD1048568" t="e" cm="1">
         <f t="array" ref="XFD1048568">solver_soc</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="1048569" spans="16384:16384" x14ac:dyDescent="0.25">
+    <row r="1048569" spans="16384:16384" x14ac:dyDescent="0.2">
       <c r="XFD1048569" t="e" cm="1">
         <f t="array" ref="XFD1048569">solver_lpt</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="1048570" spans="16384:16384" x14ac:dyDescent="0.25">
+    <row r="1048570" spans="16384:16384" x14ac:dyDescent="0.2">
       <c r="XFD1048570" t="e" cm="1">
         <f t="array" ref="XFD1048570">solver_lpp</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="1048571" spans="16384:16384" x14ac:dyDescent="0.25">
+    <row r="1048571" spans="16384:16384" x14ac:dyDescent="0.2">
       <c r="XFD1048571" t="e" cm="1">
         <f t="array" ref="XFD1048571">solver_gap</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="1048572" spans="16384:16384" x14ac:dyDescent="0.25">
+    <row r="1048572" spans="16384:16384" x14ac:dyDescent="0.2">
       <c r="XFD1048572" t="e" cm="1">
         <f t="array" ref="XFD1048572">solver_ips</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="1048573" spans="16384:16384" x14ac:dyDescent="0.25">
+    <row r="1048573" spans="16384:16384" x14ac:dyDescent="0.2">
       <c r="XFD1048573" t="e" cm="1">
         <f t="array" ref="XFD1048573">solver_fea</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="1048574" spans="16384:16384" x14ac:dyDescent="0.25">
+    <row r="1048574" spans="16384:16384" x14ac:dyDescent="0.2">
       <c r="XFD1048574" t="e" cm="1">
         <f t="array" ref="XFD1048574">solver_ipi</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="1048575" spans="16384:16384" x14ac:dyDescent="0.25">
+    <row r="1048575" spans="16384:16384" x14ac:dyDescent="0.2">
       <c r="XFD1048575" t="e" cm="1">
         <f t="array" ref="XFD1048575">solver_ipd</f>
         <v>#NAME?</v>
@@ -10427,20 +10421,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A12:B13"/>
-    <mergeCell ref="C12:E13"/>
-    <mergeCell ref="A14:E16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="C17:E18"/>
     <mergeCell ref="A29:E31"/>
     <mergeCell ref="A32:B33"/>
     <mergeCell ref="C32:E33"/>
@@ -10451,6 +10431,20 @@
     <mergeCell ref="A24:E26"/>
     <mergeCell ref="A27:B28"/>
     <mergeCell ref="C27:E28"/>
+    <mergeCell ref="A12:B13"/>
+    <mergeCell ref="C12:E13"/>
+    <mergeCell ref="A14:E16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="C17:E18"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
IBA assignment 1 done
</commit_message>
<xml_diff>
--- a/Introduction_to_Business_Analytics/Assignment/Assignment_1/IBA Assignment (2024-2025) - Data.xlsx
+++ b/Introduction_to_Business_Analytics/Assignment/Assignment_1/IBA Assignment (2024-2025) - Data.xlsx
@@ -1,69 +1,143 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hekto\Desktop\Kurser\2024-2025\Introduction_to_Business_Analytics\Assignment\Assignment_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2288CF40-CC13-4F61-9361-EE0065FC6F0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2CB4C4-55F9-49AC-B8A7-6AEB494BA2BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="893" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="893" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Name and Matriculation Number" sheetId="7" r:id="rId1"/>
     <sheet name="Q1.President’s Inn Guest" sheetId="6" r:id="rId2"/>
     <sheet name="Q2.Sales Volume" sheetId="4" r:id="rId3"/>
     <sheet name="Q3.Batteries Life Expectancy" sheetId="2" r:id="rId4"/>
-    <sheet name="Q4.Flamingo Grill" sheetId="5" r:id="rId5"/>
+    <sheet name="Q4.Flamingo Gril (NO SOLVER)" sheetId="9" r:id="rId5"/>
+    <sheet name="Q4.Flamingo Grill (Solver)" sheetId="8" r:id="rId6"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId7"/>
+  </externalReferences>
   <definedNames>
+    <definedName name="anscount" localSheetId="4" hidden="1">1</definedName>
     <definedName name="anscount" hidden="1">1</definedName>
     <definedName name="limcount" hidden="1">1</definedName>
+    <definedName name="objValue">#REF!</definedName>
+    <definedName name="sencount" localSheetId="4" hidden="1">1</definedName>
     <definedName name="sencount" hidden="1">1</definedName>
+    <definedName name="solver_adj" localSheetId="5" hidden="1">'Q4.Flamingo Grill (Solver)'!$H$4:$H$9</definedName>
     <definedName name="solver_cvg" localSheetId="4" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="5" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_drv" localSheetId="5" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="5" hidden="1">2</definedName>
     <definedName name="solver_est" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="4" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="4" hidden="1">'Q4.Flamingo Grill'!$H$13:$H$20</definedName>
-    <definedName name="solver_lhs2" localSheetId="4" hidden="1">'Q4.Flamingo Grill'!$H$13:$H$20</definedName>
-    <definedName name="solver_lhs3" localSheetId="4" hidden="1">'Q4.Flamingo Grill'!$H$13:$H$20</definedName>
-    <definedName name="solver_lhs4" localSheetId="4" hidden="1">'Q4.Flamingo Grill'!$H$13:$H$20</definedName>
+    <definedName name="solver_itr" localSheetId="5" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="4" hidden="1">'Q4.Flamingo Gril (NO SOLVER)'!$H$13:$H$20</definedName>
+    <definedName name="solver_lhs1" localSheetId="5" hidden="1">'Q4.Flamingo Grill (Solver)'!$H$13</definedName>
+    <definedName name="solver_lhs10" localSheetId="5" hidden="1">'Q4.Flamingo Grill (Solver)'!$H$22</definedName>
+    <definedName name="solver_lhs11" localSheetId="5" hidden="1">'Q4.Flamingo Grill (Solver)'!$H$23</definedName>
+    <definedName name="solver_lhs12" localSheetId="5" hidden="1">'Q4.Flamingo Grill (Solver)'!$H$4:$H$9</definedName>
+    <definedName name="solver_lhs13" localSheetId="5" hidden="1">'Q4.Flamingo Grill (Solver)'!$H$4:$H$9</definedName>
+    <definedName name="solver_lhs2" localSheetId="4" hidden="1">'Q4.Flamingo Gril (NO SOLVER)'!$H$13:$H$20</definedName>
+    <definedName name="solver_lhs2" localSheetId="5" hidden="1">'Q4.Flamingo Grill (Solver)'!$H$14</definedName>
+    <definedName name="solver_lhs3" localSheetId="4" hidden="1">'Q4.Flamingo Gril (NO SOLVER)'!$H$13:$H$20</definedName>
+    <definedName name="solver_lhs3" localSheetId="5" hidden="1">'Q4.Flamingo Grill (Solver)'!$H$15</definedName>
+    <definedName name="solver_lhs4" localSheetId="4" hidden="1">'Q4.Flamingo Gril (NO SOLVER)'!$H$13:$H$20</definedName>
+    <definedName name="solver_lhs4" localSheetId="5" hidden="1">'Q4.Flamingo Grill (Solver)'!$H$16</definedName>
+    <definedName name="solver_lhs5" localSheetId="5" hidden="1">'Q4.Flamingo Grill (Solver)'!$H$17</definedName>
+    <definedName name="solver_lhs6" localSheetId="5" hidden="1">'Q4.Flamingo Grill (Solver)'!$H$18</definedName>
+    <definedName name="solver_lhs7" localSheetId="5" hidden="1">'Q4.Flamingo Grill (Solver)'!$H$19</definedName>
+    <definedName name="solver_lhs8" localSheetId="5" hidden="1">'Q4.Flamingo Grill (Solver)'!$H$20</definedName>
+    <definedName name="solver_lhs9" localSheetId="5" hidden="1">'Q4.Flamingo Grill (Solver)'!$H$21</definedName>
     <definedName name="solver_lin" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_lin" localSheetId="5" hidden="1">2</definedName>
     <definedName name="solver_mip" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="5" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="4" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="5" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="4" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="5" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="5" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="5" hidden="1">2</definedName>
     <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="5" hidden="1">2147483647</definedName>
     <definedName name="solver_ntri" hidden="1">1000</definedName>
     <definedName name="solver_num" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_num" localSheetId="5" hidden="1">13</definedName>
     <definedName name="solver_nwt" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="5" hidden="1">'Q4.Flamingo Grill (Solver)'!$K$4</definedName>
     <definedName name="solver_pre" localSheetId="4" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="5" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_rbv" localSheetId="5" hidden="1">2</definedName>
     <definedName name="solver_rel1" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_rel1" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_rel10" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_rel11" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_rel12" localSheetId="5" hidden="1">4</definedName>
+    <definedName name="solver_rel13" localSheetId="5" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_rel2" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_rel3" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_rel3" localSheetId="5" hidden="1">3</definedName>
     <definedName name="solver_rel4" localSheetId="4" hidden="1">3</definedName>
-    <definedName name="solver_rhs1" localSheetId="4" hidden="1">'Q4.Flamingo Grill'!$I$17:$I$24</definedName>
-    <definedName name="solver_rhs2" localSheetId="4" hidden="1">'Q4.Flamingo Grill'!$I$17:$I$24</definedName>
-    <definedName name="solver_rhs3" localSheetId="4" hidden="1">'Q4.Flamingo Grill'!$I$17:$I$24</definedName>
-    <definedName name="solver_rhs4" localSheetId="4" hidden="1">'Q4.Flamingo Grill'!$I$17:$I$24</definedName>
+    <definedName name="solver_rel4" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_rel5" localSheetId="5" hidden="1">3</definedName>
+    <definedName name="solver_rel6" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_rel7" localSheetId="5" hidden="1">3</definedName>
+    <definedName name="solver_rel8" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_rel9" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_rhs1" localSheetId="4" hidden="1">'Q4.Flamingo Gril (NO SOLVER)'!$I$17:$I$24</definedName>
+    <definedName name="solver_rhs1" localSheetId="5" hidden="1">'Q4.Flamingo Grill (Solver)'!$J$13</definedName>
+    <definedName name="solver_rhs10" localSheetId="5" hidden="1">'Q4.Flamingo Grill (Solver)'!$J$22</definedName>
+    <definedName name="solver_rhs11" localSheetId="5" hidden="1">'Q4.Flamingo Grill (Solver)'!$J$22</definedName>
+    <definedName name="solver_rhs12" localSheetId="5" hidden="1">"integer"</definedName>
+    <definedName name="solver_rhs13" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_rhs2" localSheetId="4" hidden="1">'Q4.Flamingo Gril (NO SOLVER)'!$I$17:$I$24</definedName>
+    <definedName name="solver_rhs2" localSheetId="5" hidden="1">'Q4.Flamingo Grill (Solver)'!$J$14</definedName>
+    <definedName name="solver_rhs3" localSheetId="4" hidden="1">'Q4.Flamingo Gril (NO SOLVER)'!$I$17:$I$24</definedName>
+    <definedName name="solver_rhs3" localSheetId="5" hidden="1">'Q4.Flamingo Grill (Solver)'!$J$15</definedName>
+    <definedName name="solver_rhs4" localSheetId="4" hidden="1">'Q4.Flamingo Gril (NO SOLVER)'!$I$17:$I$24</definedName>
+    <definedName name="solver_rhs4" localSheetId="5" hidden="1">'Q4.Flamingo Grill (Solver)'!$J$16</definedName>
+    <definedName name="solver_rhs5" localSheetId="5" hidden="1">'Q4.Flamingo Grill (Solver)'!$J$17</definedName>
+    <definedName name="solver_rhs6" localSheetId="5" hidden="1">'Q4.Flamingo Grill (Solver)'!$J$18</definedName>
+    <definedName name="solver_rhs7" localSheetId="5" hidden="1">'Q4.Flamingo Grill (Solver)'!$J$19</definedName>
+    <definedName name="solver_rhs8" localSheetId="5" hidden="1">'Q4.Flamingo Grill (Solver)'!$J$20</definedName>
+    <definedName name="solver_rhs9" localSheetId="5" hidden="1">'Q4.Flamingo Grill (Solver)'!$J$21</definedName>
     <definedName name="solver_rlx" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="5" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_rsmp" hidden="1">2</definedName>
     <definedName name="solver_scl" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_scl" localSheetId="5" hidden="1">2</definedName>
     <definedName name="solver_seed" hidden="1">0</definedName>
     <definedName name="solver_sho" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="5" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="4" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="5" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="5" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="4" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="5" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_val" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_ver" localSheetId="5" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -106,7 +180,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="219">
   <si>
     <t>Week</t>
   </si>
@@ -642,19 +716,446 @@
     <t>The newspaper budget is to be at least $30,000.</t>
   </si>
   <si>
-    <t>Use at least twice as many radio advertisements as television advertisements. F</t>
+    <t>Rule 6</t>
+  </si>
+  <si>
+    <t>The budget has been set at $279,000</t>
+  </si>
+  <si>
+    <t>Rule 7</t>
+  </si>
+  <si>
+    <t>the advertising campaign must reach at least 100,000 new customers</t>
+  </si>
+  <si>
+    <t>Preprocess</t>
+  </si>
+  <si>
+    <t>Exposer per ad</t>
+  </si>
+  <si>
+    <t>Cost per ad</t>
+  </si>
+  <si>
+    <t>Ad amount</t>
+  </si>
+  <si>
+    <t>New customers per ad</t>
+  </si>
+  <si>
+    <t>Sum new customers</t>
+  </si>
+  <si>
+    <t>Sum cost</t>
+  </si>
+  <si>
+    <t>Sum exposer</t>
+  </si>
+  <si>
+    <t>Total budget left</t>
+  </si>
+  <si>
+    <t>Radio budget left</t>
+  </si>
+  <si>
+    <t>Budget</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use at least twice as many radio advertisements as television advertisements. </t>
+  </si>
+  <si>
+    <t>Telivion ad max</t>
+  </si>
+  <si>
+    <t>Newspaper min left</t>
+  </si>
+  <si>
+    <t>Is R &gt;= 2T</t>
+  </si>
+  <si>
+    <t>Rule 3 (10 first)</t>
+  </si>
+  <si>
+    <t>Rule 3 (4 next)</t>
+  </si>
+  <si>
+    <t>TV</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>Rule 5(10 next)</t>
+  </si>
+  <si>
+    <t>Rule 5 (20 first)</t>
+  </si>
+  <si>
+    <t>Rule 1(15 first)</t>
+  </si>
+  <si>
+    <t>Rule 1(13 next)</t>
+  </si>
+  <si>
+    <t>SUM</t>
+  </si>
+  <si>
+    <t>After preprocess</t>
+  </si>
+  <si>
+    <t>T0</t>
+  </si>
+  <si>
+    <t>N0</t>
+  </si>
+  <si>
+    <t>R0</t>
+  </si>
+  <si>
+    <t>max(T1)</t>
+  </si>
+  <si>
+    <t>max(R1)</t>
+  </si>
+  <si>
+    <t>Math 
+( An optimal solution to a linear programming problem can be found at an extreme point of the feasible region for the problem)</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Nsum = X +X0
+Tsum = T +T0
+Rsum = R +R0
+N0 = 30 
+T0 = 14
+R0= 28
+Objective = Z = 55T+ 20R + 5N
+Constrains:
+X,T,R </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>ϵ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Z ˄ X,T,R </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>≥</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 0
+3000R + 10000T + 1000N ≤ 25000
+R ≥  2T
+T ≤ 6
+R </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>≤</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">  5  | (15000/3000)
+T=0
+3000R + 1000N = 15000  | R  ≥ 2 *0
+T = 0, N = 0
+3000R = 15000  
+R= 15000/ 3000 = 5
+T = 0, R = 0  | 0 ≥ 2 *0
+1000N = 15000  
+N = 15
+T=1
+3000R + 10000 + 1000N = 25000  | R  ≥ 2 *1
+T=1, N=0
+ 3000R = 15000
+R=5
+T=1, R=2
+6000 + 10000 + 1000N = 25000
+1000N = 9000
+N = 9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Total =  (55T+ 20R + 5N)+ (55T</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>0x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>+ 20R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>0x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>+ 5N</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>0x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>) + (90T</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>0y</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>+ 25R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>0y</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>+ 10N</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>0y</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>0x</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>0x</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>0x</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>0y</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>0y</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>0y</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">(55T0x+ 20R0x+ 5N0x) + (90T0y+ 25R0y+ 10N0y) </t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Radio Budget</t>
+  </si>
+  <si>
+    <t>Television ad max</t>
+  </si>
+  <si>
+    <t>Newspapper min bud</t>
+  </si>
+  <si>
+    <t>Constains:</t>
+  </si>
+  <si>
+    <t>&lt;=</t>
+  </si>
+  <si>
+    <t>No more then 10 TV ads with 90 exposure</t>
+  </si>
+  <si>
+    <t>No more then 15 radio ads with 25 exposure</t>
+  </si>
+  <si>
+    <t>No more then 20 newspaper ads with 10 exposure</t>
+  </si>
+  <si>
+    <t>&gt;=</t>
+  </si>
+  <si>
+    <t>Television Minimum bud</t>
+  </si>
+  <si>
+    <t>All decision variables are positive integers X,T,R ϵ Z ˄ X,T,R ≥ 0</t>
+  </si>
+  <si>
+    <t>"You must conduct all the calculations using Excel or its built-in functions", Solver is a add-in(but pre installed) so did both calculations by hand and via solver as was unsure what was the criteria.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="3">
+  <numFmts count="6">
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="166" formatCode="[$$-409]#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="168" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -675,13 +1176,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -820,8 +1314,24 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -876,8 +1386,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="62">
+  <borders count="67">
     <border>
       <left/>
       <right/>
@@ -1610,109 +2132,167 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="189">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="7" applyFont="1"/>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="7" applyFont="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="23" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="23" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="23" xfId="4" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="6" fillId="2" borderId="23" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="23" xfId="4" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="23" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="23" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="23" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="23" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="23" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="24" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="4" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="6" fillId="2" borderId="24" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="24" xfId="4" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="24" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="24" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="24" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="24" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="7" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="7" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="4" borderId="25" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="26" xfId="6" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="6" fillId="4" borderId="27" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="28" xfId="6" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="6" fillId="4" borderId="29" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="30" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="31" xfId="6" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="6" fillId="4" borderId="32" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="4" borderId="25" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="26" xfId="6" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="5" fillId="4" borderId="27" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="28" xfId="6" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="5" fillId="4" borderId="29" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="30" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="31" xfId="6" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="5" fillId="4" borderId="32" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="6" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="6" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1724,109 +2304,85 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="36" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="36" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="37" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="37" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="36" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="36" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="37" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="37" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="39" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="43" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="44" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="40" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="41" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="38" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="48" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="49" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="49" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="50" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="50" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="51" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="51" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="34" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1835,164 +2391,321 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="33" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="57" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="57" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="61" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="61" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="58" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="58" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="57" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="57" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="58" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="58" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="54" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="54" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="55" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="55" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="56" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="56" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="58" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="58" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="58" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="58" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="59" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="59" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="60" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="60" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="46" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="47" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="47" xfId="11" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="46" xfId="11" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="43" xfId="11" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="11" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="41" xfId="11" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="48" xfId="12" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="44" xfId="11" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="38" xfId="11" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="39" xfId="12" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="40" xfId="11" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="12" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="13"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="14"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="13" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="57" xfId="13" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="13" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="58" xfId="13" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="57" xfId="13" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="57" xfId="13" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="13" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="57" xfId="13" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="61" xfId="13" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="13" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="62" xfId="13" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="58" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="58" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="66" xfId="13" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="65" xfId="13" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="6" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="13" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="62" xfId="13" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="61" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="10" borderId="61" xfId="13" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="61" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="64" xfId="13" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="63" xfId="13" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="57" xfId="15" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="13" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="13" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="40" xfId="13" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="41" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="40" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="40" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="48" xfId="13" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="13" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="13" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="39" xfId="13" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="13" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="3" xfId="13" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="43" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="42" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="13" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="6" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="16">
     <cellStyle name="40% - Accent1" xfId="4" builtinId="31"/>
+    <cellStyle name="40% - Accent1 2" xfId="11" xr:uid="{AA59DACE-63B5-495F-B9D4-CD86FD0B45FF}"/>
     <cellStyle name="40% - Accent2" xfId="5" builtinId="35"/>
     <cellStyle name="40% - Accent3" xfId="6" builtinId="39"/>
+    <cellStyle name="40% - Accent3 2" xfId="12" xr:uid="{C08283F8-F5EC-42C7-99A8-AB85FF7F2E49}"/>
     <cellStyle name="Currency 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Currency 2 2" xfId="15" xr:uid="{6AC85918-FB99-4FC2-B03F-D15AE7E29D76}"/>
     <cellStyle name="Currency 3" xfId="8" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 2 2" xfId="13" xr:uid="{7037CDD5-4B72-4379-AF66-50B96F0DD3CA}"/>
     <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="Normal 4" xfId="7" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal 5" xfId="14" xr:uid="{56875F12-92D4-4A19-BA5E-5F47A4C05655}"/>
     <cellStyle name="Normal_Sheet2" xfId="10" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
     <cellStyle name="Percent 2" xfId="9" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
   </cellStyles>
@@ -2724,6 +3437,30 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Portfolio Selection"/>
+      <sheetName val="Blending Problem"/>
+      <sheetName val="Marketing Research"/>
+      <sheetName val="Media Selection"/>
+      <sheetName val="Q4.Flamingo Gril (NO SOLVER)"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
@@ -3093,10 +3830,10 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:3" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="88" t="s">
+      <c r="B6" s="80" t="s">
         <v>111</v>
       </c>
-      <c r="C6" s="88"/>
+      <c r="C6" s="80"/>
     </row>
     <row r="7" spans="2:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B7" s="33"/>
@@ -3123,6 +3860,18 @@
     <mergeCell ref="B6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{F7C9EE02-42E1-4005-9D12-6889AFFD525C}">
+      <x15:webExtensions xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x15:webExtension appRef="{83B5D8B2-AF49-6D41-B7BB-A01E4097B078}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{A0C87E43-B8AD-0641-A98E-254343A9F0BF}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+      </x15:webExtensions>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4471,115 +5220,115 @@
   <sheetData>
     <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J14" s="95" t="s">
+      <c r="J14" s="87" t="s">
         <v>138</v>
       </c>
-      <c r="K14" s="96"/>
-      <c r="L14" s="96"/>
-      <c r="M14" s="96"/>
-      <c r="N14" s="96"/>
-      <c r="O14" s="97"/>
-      <c r="P14" s="103"/>
-      <c r="Q14" s="95" t="s">
+      <c r="K14" s="88"/>
+      <c r="L14" s="88"/>
+      <c r="M14" s="88"/>
+      <c r="N14" s="88"/>
+      <c r="O14" s="89"/>
+      <c r="P14" s="95"/>
+      <c r="Q14" s="87" t="s">
         <v>139</v>
       </c>
-      <c r="R14" s="96"/>
-      <c r="S14" s="97"/>
+      <c r="R14" s="88"/>
+      <c r="S14" s="89"/>
     </row>
     <row r="15" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="108" t="s">
+      <c r="A15" s="100" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="105" t="s">
+      <c r="B15" s="97" t="s">
         <v>113</v>
       </c>
-      <c r="C15" s="111" t="s">
+      <c r="C15" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="112"/>
-      <c r="E15" s="113"/>
-      <c r="F15" s="114" t="s">
+      <c r="D15" s="104"/>
+      <c r="E15" s="105"/>
+      <c r="F15" s="106" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="115"/>
-      <c r="H15" s="116"/>
-      <c r="J15" s="98"/>
-      <c r="K15" s="99"/>
-      <c r="L15" s="99"/>
-      <c r="M15" s="99"/>
-      <c r="N15" s="99"/>
-      <c r="O15" s="100"/>
-      <c r="P15" s="104"/>
-      <c r="Q15" s="98"/>
-      <c r="R15" s="99"/>
-      <c r="S15" s="100"/>
+      <c r="G15" s="107"/>
+      <c r="H15" s="108"/>
+      <c r="J15" s="90"/>
+      <c r="K15" s="91"/>
+      <c r="L15" s="91"/>
+      <c r="M15" s="91"/>
+      <c r="N15" s="91"/>
+      <c r="O15" s="92"/>
+      <c r="P15" s="96"/>
+      <c r="Q15" s="90"/>
+      <c r="R15" s="91"/>
+      <c r="S15" s="92"/>
     </row>
     <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="109"/>
-      <c r="B16" s="106"/>
-      <c r="C16" s="117" t="s">
+      <c r="A16" s="101"/>
+      <c r="B16" s="98"/>
+      <c r="C16" s="109" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="119" t="s">
+      <c r="D16" s="111" t="s">
         <v>115</v>
       </c>
-      <c r="E16" s="121" t="s">
+      <c r="E16" s="113" t="s">
         <v>114</v>
       </c>
-      <c r="F16" s="117" t="s">
+      <c r="F16" s="109" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="119" t="s">
+      <c r="G16" s="111" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="121" t="s">
+      <c r="H16" s="113" t="s">
         <v>11</v>
       </c>
-      <c r="J16" s="93" t="s">
+      <c r="J16" s="85" t="s">
         <v>7</v>
       </c>
-      <c r="K16" s="93" t="s">
+      <c r="K16" s="85" t="s">
         <v>115</v>
       </c>
-      <c r="L16" s="93" t="s">
+      <c r="L16" s="85" t="s">
         <v>114</v>
       </c>
-      <c r="M16" s="93" t="s">
+      <c r="M16" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="N16" s="93" t="s">
+      <c r="N16" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="O16" s="93" t="s">
+      <c r="O16" s="85" t="s">
         <v>11</v>
       </c>
-      <c r="P16" s="102"/>
-      <c r="Q16" s="101" t="str">
+      <c r="P16" s="94"/>
+      <c r="Q16" s="93" t="str">
         <f>INDEX(J16:O16, MATCH(Q18, J18:O18, 0))</f>
         <v>α=0.25</v>
       </c>
-      <c r="R16" s="101"/>
-      <c r="S16" s="101"/>
+      <c r="R16" s="93"/>
+      <c r="S16" s="93"/>
     </row>
     <row r="17" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="110"/>
-      <c r="B17" s="107"/>
-      <c r="C17" s="118"/>
-      <c r="D17" s="120"/>
-      <c r="E17" s="122"/>
-      <c r="F17" s="118"/>
-      <c r="G17" s="120"/>
-      <c r="H17" s="122"/>
-      <c r="J17" s="94"/>
-      <c r="K17" s="94"/>
-      <c r="L17" s="94"/>
-      <c r="M17" s="94"/>
-      <c r="N17" s="94"/>
-      <c r="O17" s="94"/>
-      <c r="P17" s="92"/>
-      <c r="Q17" s="89"/>
-      <c r="R17" s="89"/>
-      <c r="S17" s="89"/>
+      <c r="A17" s="102"/>
+      <c r="B17" s="99"/>
+      <c r="C17" s="110"/>
+      <c r="D17" s="112"/>
+      <c r="E17" s="114"/>
+      <c r="F17" s="110"/>
+      <c r="G17" s="112"/>
+      <c r="H17" s="114"/>
+      <c r="J17" s="86"/>
+      <c r="K17" s="86"/>
+      <c r="L17" s="86"/>
+      <c r="M17" s="86"/>
+      <c r="N17" s="86"/>
+      <c r="O17" s="86"/>
+      <c r="P17" s="84"/>
+      <c r="Q17" s="81"/>
+      <c r="R17" s="81"/>
+      <c r="S17" s="81"/>
     </row>
     <row r="18" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="48">
@@ -4594,37 +5343,37 @@
       <c r="F18" s="37"/>
       <c r="G18" s="40"/>
       <c r="H18" s="41"/>
-      <c r="J18" s="90">
+      <c r="J18" s="82">
         <f>SUMXMY2(B22:B173,C22:C173)/COUNT(C22:C173)</f>
         <v>222.94202302631578</v>
       </c>
-      <c r="K18" s="90">
+      <c r="K18" s="82">
         <f>SUMXMY2(B23:B173,D23:D173)/COUNT(D23:D173)</f>
         <v>215.94172185430466</v>
       </c>
-      <c r="L18" s="90">
+      <c r="L18" s="82">
         <f>SUMXMY2(B24:B173,E24:E173)/COUNT(E24:E173)</f>
         <v>213.54296296296289</v>
       </c>
-      <c r="M18" s="90">
+      <c r="M18" s="82">
         <f>SUMXMY2($B$19:$B$173,F19:F173)/COUNT(F19:F173)</f>
         <v>201.60269314672905</v>
       </c>
-      <c r="N18" s="90">
+      <c r="N18" s="82">
         <f>SUMXMY2($B$19:$B$173,G19:G173)/COUNT(G19:G173)</f>
         <v>233.95925875075537</v>
       </c>
-      <c r="O18" s="90">
+      <c r="O18" s="82">
         <f>SUMXMY2($B$19:$B$173,H19:H173)/COUNT(H19:H173)</f>
         <v>273.77003808044924</v>
       </c>
-      <c r="P18" s="92"/>
-      <c r="Q18" s="89">
+      <c r="P18" s="84"/>
+      <c r="Q18" s="81">
         <f>MIN(J18:O18)</f>
         <v>201.60269314672905</v>
       </c>
-      <c r="R18" s="89"/>
-      <c r="S18" s="89"/>
+      <c r="R18" s="81"/>
+      <c r="S18" s="81"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="50">
@@ -4648,16 +5397,16 @@
         <f>0.75*B18+0.25*B18</f>
         <v>136</v>
       </c>
-      <c r="J19" s="91"/>
-      <c r="K19" s="91"/>
-      <c r="L19" s="91"/>
-      <c r="M19" s="91"/>
-      <c r="N19" s="91"/>
-      <c r="O19" s="91"/>
-      <c r="P19" s="92"/>
-      <c r="Q19" s="89"/>
-      <c r="R19" s="89"/>
-      <c r="S19" s="89"/>
+      <c r="J19" s="83"/>
+      <c r="K19" s="83"/>
+      <c r="L19" s="83"/>
+      <c r="M19" s="83"/>
+      <c r="N19" s="83"/>
+      <c r="O19" s="83"/>
+      <c r="P19" s="84"/>
+      <c r="Q19" s="81"/>
+      <c r="R19" s="81"/>
+      <c r="S19" s="81"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="50">
@@ -9565,27 +10314,27 @@
         <v>157</v>
       </c>
       <c r="B174" s="55"/>
-      <c r="C174" s="83">
+      <c r="C174" s="73">
         <f>AVERAGE(B170:B173)</f>
         <v>127.25</v>
       </c>
-      <c r="D174" s="84">
+      <c r="D174" s="74">
         <f>AVERAGE(B169:B173)</f>
         <v>133</v>
       </c>
-      <c r="E174" s="85">
+      <c r="E174" s="75">
         <f>AVERAGE(B168:B173)</f>
         <v>132.33333333333334</v>
       </c>
-      <c r="F174" s="83">
+      <c r="F174" s="73">
         <f>0.25*B173+0.75*F173</f>
         <v>131.26287997157061</v>
       </c>
-      <c r="G174" s="84">
+      <c r="G174" s="74">
         <f>0.5*B173+0.5*G173</f>
         <v>126.50666526296413</v>
       </c>
-      <c r="H174" s="85">
+      <c r="H174" s="75">
         <f>0.75*B173+0.25*H173</f>
         <v>124.6787609620504</v>
       </c>
@@ -9682,7 +10431,7 @@
     <mergeCell ref="O18:O19"/>
     <mergeCell ref="P18:P19"/>
   </mergeCells>
-  <phoneticPr fontId="24" type="noConversion"/>
+  <phoneticPr fontId="23" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -9693,8 +10442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B4:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -9735,10 +10484,10 @@
       <c r="B10" s="5"/>
     </row>
     <row r="11" spans="2:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="123" t="s">
+      <c r="B11" s="115" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="87" t="s">
+      <c r="C11" s="77" t="s">
         <v>140</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -9746,8 +10495,8 @@
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="123"/>
-      <c r="C12" s="86" t="s">
+      <c r="B12" s="115"/>
+      <c r="C12" s="76" t="s">
         <v>141</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -9810,7 +10559,7 @@
       <c r="B20" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="136" t="s">
+      <c r="C20" s="78" t="s">
         <v>150</v>
       </c>
     </row>
@@ -9875,552 +10624,1937 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A2:XFD1048575"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{607188CE-3FF0-4065-8320-0AA4B52A5C60}">
+  <dimension ref="A1:RQH1048575"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="71" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:B18"/>
+    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="R36" sqref="R36:R40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" customWidth="1"/>
-    <col min="7" max="7" width="37.140625" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" customWidth="1"/>
-    <col min="11" max="11" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="12.42578125" style="134" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="134" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="134" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" style="134" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="134"/>
+    <col min="7" max="7" width="37.140625" style="134" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" style="134" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" style="134"/>
+    <col min="10" max="12" width="20.7109375" style="134" customWidth="1"/>
+    <col min="13" max="15" width="10.7109375" style="134" customWidth="1"/>
+    <col min="16" max="27" width="20.7109375" style="134" customWidth="1"/>
+    <col min="28" max="28" width="20.7109375" style="135" customWidth="1"/>
+    <col min="29" max="30" width="8.85546875" style="135"/>
+    <col min="31" max="31" width="8.42578125" style="135" customWidth="1"/>
+    <col min="32" max="12617" width="8.85546875" style="135"/>
+    <col min="12618" max="12618" width="8.85546875" style="134"/>
+    <col min="12619" max="16384" width="8.85546875" style="135"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="G2" s="128"/>
-      <c r="H2" s="128"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="59"/>
-    </row>
-    <row r="3" spans="1:12" ht="47.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="130" t="s">
+    <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="188" t="s">
+        <v>218</v>
+      </c>
+      <c r="B1" s="188"/>
+      <c r="C1" s="188"/>
+      <c r="D1" s="188"/>
+      <c r="E1" s="188"/>
+      <c r="F1" s="188"/>
+      <c r="G1" s="188"/>
+      <c r="H1" s="188"/>
+      <c r="I1" s="188"/>
+      <c r="J1" s="188"/>
+      <c r="K1" s="188"/>
+      <c r="L1" s="188"/>
+      <c r="M1" s="188"/>
+      <c r="N1" s="188"/>
+      <c r="O1" s="188"/>
+      <c r="P1" s="188"/>
+      <c r="Q1" s="188"/>
+      <c r="R1" s="188"/>
+      <c r="S1" s="188"/>
+    </row>
+    <row r="2" spans="1:24" s="134" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="188"/>
+      <c r="B2" s="188"/>
+      <c r="C2" s="188"/>
+      <c r="D2" s="188"/>
+      <c r="E2" s="188"/>
+      <c r="F2" s="188"/>
+      <c r="G2" s="188"/>
+      <c r="H2" s="188"/>
+      <c r="I2" s="188"/>
+      <c r="J2" s="188"/>
+      <c r="K2" s="188"/>
+      <c r="L2" s="188"/>
+      <c r="M2" s="188"/>
+      <c r="N2" s="188"/>
+      <c r="O2" s="188"/>
+      <c r="P2" s="188"/>
+      <c r="Q2" s="188"/>
+      <c r="R2" s="188"/>
+      <c r="S2" s="188"/>
+    </row>
+    <row r="3" spans="1:24" s="134" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="182" t="s">
         <v>116</v>
       </c>
-      <c r="B3" s="130"/>
-      <c r="C3" s="60" t="s">
+      <c r="B3" s="182"/>
+      <c r="C3" s="177" t="s">
         <v>117</v>
       </c>
-      <c r="D3" s="60" t="s">
+      <c r="D3" s="177" t="s">
         <v>118</v>
       </c>
-      <c r="E3" s="60" t="s">
+      <c r="E3" s="177" t="s">
         <v>119</v>
       </c>
-      <c r="F3" s="58"/>
-      <c r="G3" s="129" t="s">
+      <c r="F3" s="162"/>
+      <c r="G3" s="181" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="129"/>
-      <c r="I3" s="58"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="61" t="s">
+      <c r="H3" s="181"/>
+      <c r="I3" s="162"/>
+      <c r="J3" s="177"/>
+      <c r="K3" s="180" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="131" t="s">
+    <row r="4" spans="1:24" s="134" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="179" t="s">
         <v>120</v>
       </c>
-      <c r="B4" s="81" t="s">
+      <c r="B4" s="178" t="s">
         <v>130</v>
       </c>
-      <c r="C4" s="66">
+      <c r="C4" s="124">
         <v>90</v>
       </c>
-      <c r="D4" s="67">
+      <c r="D4" s="129">
         <v>4000</v>
       </c>
-      <c r="E4" s="126">
+      <c r="E4" s="123">
         <v>10000</v>
       </c>
-      <c r="F4" s="58"/>
-      <c r="G4" s="56" t="s">
+      <c r="F4" s="162"/>
+      <c r="G4" s="174" t="s">
         <v>123</v>
       </c>
-      <c r="H4" s="76"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="60" t="s">
+      <c r="H4" s="133">
+        <f>M18</f>
+        <v>10</v>
+      </c>
+      <c r="I4" s="162"/>
+      <c r="J4" s="177" t="s">
         <v>129</v>
       </c>
-      <c r="K4" s="62"/>
-    </row>
-    <row r="5" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="125"/>
-      <c r="B5" s="68" t="s">
+      <c r="K4" s="176">
+        <f>W40</f>
+        <v>2160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" s="134" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="168"/>
+      <c r="B5" s="175" t="s">
         <v>133</v>
       </c>
-      <c r="C5" s="69">
+      <c r="C5" s="132">
         <v>55</v>
       </c>
-      <c r="D5" s="70">
+      <c r="D5" s="126">
         <v>1500</v>
       </c>
-      <c r="E5" s="127"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="56" t="s">
+      <c r="E5" s="122"/>
+      <c r="F5" s="162"/>
+      <c r="G5" s="174" t="s">
         <v>125</v>
       </c>
-      <c r="H5" s="63"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="58"/>
-      <c r="K5" s="58"/>
-    </row>
-    <row r="6" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="124" t="s">
+      <c r="H5" s="131">
+        <f>J20+S40</f>
+        <v>5</v>
+      </c>
+      <c r="I5" s="162"/>
+      <c r="J5" s="162"/>
+      <c r="K5" s="162"/>
+    </row>
+    <row r="6" spans="1:24" s="134" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="172" t="s">
         <v>121</v>
       </c>
-      <c r="B6" s="65" t="s">
+      <c r="B6" s="171" t="s">
         <v>131</v>
       </c>
-      <c r="C6" s="71">
+      <c r="C6" s="130">
         <v>25</v>
       </c>
-      <c r="D6" s="67">
+      <c r="D6" s="129">
         <v>2000</v>
       </c>
-      <c r="E6" s="126">
+      <c r="E6" s="123">
         <v>3000</v>
       </c>
-      <c r="F6" s="58"/>
-      <c r="G6" s="79" t="s">
+      <c r="F6" s="162"/>
+      <c r="G6" s="170" t="s">
         <v>124</v>
       </c>
-      <c r="H6" s="77"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="58"/>
-      <c r="K6" s="58"/>
-    </row>
-    <row r="7" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="125"/>
-      <c r="B7" s="82" t="s">
+      <c r="H6" s="128">
+        <f>N26</f>
+        <v>15</v>
+      </c>
+      <c r="I6" s="162"/>
+      <c r="J6" s="162"/>
+      <c r="K6" s="162"/>
+    </row>
+    <row r="7" spans="1:24" s="134" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="168"/>
+      <c r="B7" s="167" t="s">
         <v>132</v>
       </c>
-      <c r="C7" s="72">
+      <c r="C7" s="127">
         <v>20</v>
       </c>
-      <c r="D7" s="70">
+      <c r="D7" s="126">
         <v>1200</v>
       </c>
-      <c r="E7" s="127"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="56" t="s">
+      <c r="E7" s="122"/>
+      <c r="F7" s="162"/>
+      <c r="G7" s="174" t="s">
         <v>126</v>
       </c>
-      <c r="H7" s="80"/>
-      <c r="I7" s="58"/>
-      <c r="J7" s="58"/>
-      <c r="K7" s="58"/>
-    </row>
-    <row r="8" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="124" t="s">
+      <c r="H7" s="173">
+        <f>N28+T40</f>
+        <v>18</v>
+      </c>
+      <c r="I7" s="162"/>
+      <c r="J7" s="162"/>
+      <c r="K7" s="162"/>
+    </row>
+    <row r="8" spans="1:24" s="134" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="172" t="s">
         <v>122</v>
       </c>
-      <c r="B8" s="65" t="s">
+      <c r="B8" s="171" t="s">
         <v>134</v>
       </c>
-      <c r="C8" s="73">
+      <c r="C8" s="125">
         <v>10</v>
       </c>
-      <c r="D8" s="66">
+      <c r="D8" s="124">
         <v>1000</v>
       </c>
-      <c r="E8" s="126">
+      <c r="E8" s="123">
         <v>1000</v>
       </c>
-      <c r="F8" s="58"/>
-      <c r="G8" s="79" t="s">
+      <c r="F8" s="162"/>
+      <c r="G8" s="170" t="s">
         <v>127</v>
       </c>
-      <c r="H8" s="78"/>
-      <c r="I8" s="58"/>
-      <c r="J8" s="58"/>
-      <c r="K8" s="58"/>
-    </row>
-    <row r="9" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="125"/>
-      <c r="B9" s="82" t="s">
+      <c r="H8" s="169">
+        <f>O22</f>
+        <v>20</v>
+      </c>
+      <c r="I8" s="162"/>
+      <c r="J8" s="162"/>
+      <c r="K8" s="162"/>
+    </row>
+    <row r="9" spans="1:24" s="134" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="168"/>
+      <c r="B9" s="167" t="s">
         <v>135</v>
       </c>
-      <c r="C9" s="74">
+      <c r="C9" s="166">
         <v>5</v>
       </c>
-      <c r="D9" s="75">
+      <c r="D9" s="165">
         <v>800</v>
       </c>
-      <c r="E9" s="127"/>
-      <c r="F9" s="58"/>
-      <c r="G9" s="57" t="s">
+      <c r="E9" s="122"/>
+      <c r="F9" s="162"/>
+      <c r="G9" s="164" t="s">
         <v>128</v>
       </c>
-      <c r="H9" s="64"/>
-      <c r="I9" s="58"/>
-      <c r="J9" s="58"/>
-      <c r="K9" s="58"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="132" t="s">
+      <c r="H9" s="163">
+        <f>O24+U40</f>
+        <v>10</v>
+      </c>
+      <c r="I9" s="162"/>
+      <c r="J9" s="162"/>
+      <c r="K9" s="162"/>
+    </row>
+    <row r="10" spans="1:24" s="134" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="J10" s="134" t="s">
+        <v>199</v>
+      </c>
+      <c r="K10" s="134" t="s">
+        <v>200</v>
+      </c>
+      <c r="L10" s="134" t="s">
+        <v>201</v>
+      </c>
+      <c r="M10" s="134" t="s">
+        <v>202</v>
+      </c>
+      <c r="N10" s="134" t="s">
+        <v>203</v>
+      </c>
+      <c r="O10" s="134" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="J11" s="134">
+        <f>R18</f>
+        <v>900</v>
+      </c>
+      <c r="K11" s="134">
+        <f>R22</f>
+        <v>200</v>
+      </c>
+      <c r="L11" s="134">
+        <f>R26</f>
+        <v>375</v>
+      </c>
+      <c r="M11" s="134">
+        <f>R20</f>
+        <v>220</v>
+      </c>
+      <c r="N11" s="134">
+        <f>R24</f>
+        <v>50</v>
+      </c>
+      <c r="O11" s="134">
+        <f>R28</f>
+        <v>260</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="138" t="s">
         <v>151</v>
       </c>
-      <c r="B12" s="133"/>
-      <c r="C12" s="133"/>
-      <c r="D12" s="133"/>
-      <c r="E12" s="133"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="133"/>
-      <c r="B13" s="133"/>
-      <c r="C13" s="133"/>
-      <c r="D13" s="133"/>
-      <c r="E13" s="133"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="134" t="s">
+      <c r="B12" s="138"/>
+      <c r="C12" s="138"/>
+      <c r="D12" s="138"/>
+      <c r="E12" s="138"/>
+    </row>
+    <row r="13" spans="1:24" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="138"/>
+      <c r="B13" s="138"/>
+      <c r="C13" s="138"/>
+      <c r="D13" s="138"/>
+      <c r="E13" s="138"/>
+    </row>
+    <row r="14" spans="1:24" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="161" t="s">
+        <v>175</v>
+      </c>
+      <c r="B14" s="161"/>
+      <c r="C14" s="161"/>
+      <c r="D14" s="161"/>
+      <c r="E14" s="161"/>
+      <c r="G14" s="137" t="s">
+        <v>164</v>
+      </c>
+      <c r="H14" s="137"/>
+      <c r="I14" s="144"/>
+      <c r="J14" s="137" t="s">
+        <v>167</v>
+      </c>
+      <c r="K14" s="137" t="s">
+        <v>166</v>
+      </c>
+      <c r="L14" s="137" t="s">
+        <v>165</v>
+      </c>
+      <c r="M14" s="144" t="s">
+        <v>181</v>
+      </c>
+      <c r="N14" s="144" t="s">
+        <v>121</v>
+      </c>
+      <c r="O14" s="144" t="s">
+        <v>122</v>
+      </c>
+      <c r="P14" s="137" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q14" s="137" t="s">
+        <v>170</v>
+      </c>
+      <c r="R14" s="137" t="s">
+        <v>171</v>
+      </c>
+      <c r="S14" s="137" t="s">
+        <v>169</v>
+      </c>
+      <c r="T14" s="137" t="s">
+        <v>177</v>
+      </c>
+      <c r="U14" s="137" t="s">
+        <v>172</v>
+      </c>
+      <c r="V14" s="137" t="s">
+        <v>173</v>
+      </c>
+      <c r="W14" s="137" t="s">
+        <v>176</v>
+      </c>
+      <c r="X14" s="137" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="161"/>
+      <c r="B15" s="161"/>
+      <c r="C15" s="161"/>
+      <c r="D15" s="161"/>
+      <c r="E15" s="161"/>
+      <c r="G15" s="137"/>
+      <c r="H15" s="137"/>
+      <c r="I15" s="142"/>
+      <c r="J15" s="137"/>
+      <c r="K15" s="137"/>
+      <c r="L15" s="137"/>
+      <c r="M15" s="139"/>
+      <c r="N15" s="139"/>
+      <c r="O15" s="139"/>
+      <c r="P15" s="137"/>
+      <c r="Q15" s="137"/>
+      <c r="R15" s="137"/>
+      <c r="S15" s="137"/>
+      <c r="T15" s="137"/>
+      <c r="U15" s="137"/>
+      <c r="V15" s="137"/>
+      <c r="W15" s="137"/>
+      <c r="X15" s="137"/>
+    </row>
+    <row r="16" spans="1:24" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="161"/>
+      <c r="B16" s="161"/>
+      <c r="C16" s="161"/>
+      <c r="D16" s="161"/>
+      <c r="E16" s="161"/>
+      <c r="G16" s="137" t="s">
+        <v>174</v>
+      </c>
+      <c r="H16" s="137"/>
+      <c r="I16" s="142"/>
+      <c r="J16" s="137"/>
+      <c r="K16" s="143"/>
+      <c r="L16" s="137"/>
+      <c r="M16" s="144"/>
+      <c r="N16" s="144"/>
+      <c r="O16" s="144"/>
+      <c r="P16" s="137"/>
+      <c r="Q16" s="143"/>
+      <c r="R16" s="137"/>
+      <c r="S16" s="137"/>
+      <c r="T16" s="160">
+        <v>30000</v>
+      </c>
+      <c r="U16" s="143">
+        <v>279000</v>
+      </c>
+      <c r="V16" s="143">
+        <v>99000</v>
+      </c>
+      <c r="W16" s="137">
+        <v>20</v>
+      </c>
+      <c r="X16" s="137"/>
+    </row>
+    <row r="17" spans="1:24" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="138" t="s">
+        <v>152</v>
+      </c>
+      <c r="B17" s="138"/>
+      <c r="C17" s="138"/>
+      <c r="D17" s="138"/>
+      <c r="E17" s="138"/>
+      <c r="G17" s="137"/>
+      <c r="H17" s="137"/>
+      <c r="I17" s="142"/>
+      <c r="J17" s="137"/>
+      <c r="K17" s="143"/>
+      <c r="L17" s="137"/>
+      <c r="M17" s="139"/>
+      <c r="N17" s="139"/>
+      <c r="O17" s="139"/>
+      <c r="P17" s="137"/>
+      <c r="Q17" s="143"/>
+      <c r="R17" s="137"/>
+      <c r="S17" s="137"/>
+      <c r="T17" s="160"/>
+      <c r="U17" s="143"/>
+      <c r="V17" s="143"/>
+      <c r="W17" s="137"/>
+      <c r="X17" s="137"/>
+    </row>
+    <row r="18" spans="1:24" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="138"/>
+      <c r="B18" s="138"/>
+      <c r="C18" s="138"/>
+      <c r="D18" s="138"/>
+      <c r="E18" s="138"/>
+      <c r="G18" s="137" t="s">
+        <v>179</v>
+      </c>
+      <c r="H18" s="137"/>
+      <c r="I18" s="142"/>
+      <c r="J18" s="137">
+        <v>10</v>
+      </c>
+      <c r="K18" s="143">
+        <f>E4</f>
+        <v>10000</v>
+      </c>
+      <c r="L18" s="137">
+        <f>C4</f>
+        <v>90</v>
+      </c>
+      <c r="M18" s="144">
+        <v>10</v>
+      </c>
+      <c r="N18" s="144"/>
+      <c r="O18" s="144"/>
+      <c r="P18" s="137">
+        <f>D4</f>
+        <v>4000</v>
+      </c>
+      <c r="Q18" s="143">
+        <f>J18*K18</f>
+        <v>100000</v>
+      </c>
+      <c r="R18" s="137">
+        <f>J18*L18</f>
+        <v>900</v>
+      </c>
+      <c r="S18" s="137">
+        <f>J18*P18</f>
+        <v>40000</v>
+      </c>
+      <c r="T18" s="143">
+        <f>T16-O18*K18</f>
+        <v>30000</v>
+      </c>
+      <c r="U18" s="143">
+        <f>U16-Q18</f>
+        <v>179000</v>
+      </c>
+      <c r="V18" s="143">
+        <f>V16-N18*K18</f>
+        <v>99000</v>
+      </c>
+      <c r="W18" s="137">
+        <f>W16-M18</f>
+        <v>10</v>
+      </c>
+      <c r="X18" s="137" t="b">
+        <f>IF(SUM($N$16:N19)&gt;=2*SUM($M$16:M19),TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="138" t="s">
+        <v>156</v>
+      </c>
+      <c r="B19" s="138"/>
+      <c r="C19" s="138"/>
+      <c r="D19" s="138"/>
+      <c r="E19" s="138"/>
+      <c r="G19" s="137"/>
+      <c r="H19" s="137"/>
+      <c r="I19" s="142"/>
+      <c r="J19" s="137"/>
+      <c r="K19" s="143"/>
+      <c r="L19" s="137"/>
+      <c r="M19" s="139"/>
+      <c r="N19" s="139"/>
+      <c r="O19" s="139"/>
+      <c r="P19" s="137"/>
+      <c r="Q19" s="143"/>
+      <c r="R19" s="137"/>
+      <c r="S19" s="137"/>
+      <c r="T19" s="137"/>
+      <c r="U19" s="137"/>
+      <c r="V19" s="137"/>
+      <c r="W19" s="137"/>
+      <c r="X19" s="137"/>
+    </row>
+    <row r="20" spans="1:24" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="138"/>
+      <c r="B20" s="138"/>
+      <c r="C20" s="138"/>
+      <c r="D20" s="138"/>
+      <c r="E20" s="138"/>
+      <c r="G20" s="137" t="s">
+        <v>180</v>
+      </c>
+      <c r="H20" s="137"/>
+      <c r="I20" s="142"/>
+      <c r="J20" s="137">
+        <v>4</v>
+      </c>
+      <c r="K20" s="143">
+        <f>E4</f>
+        <v>10000</v>
+      </c>
+      <c r="L20" s="137">
+        <f>C5</f>
+        <v>55</v>
+      </c>
+      <c r="M20" s="144">
+        <v>4</v>
+      </c>
+      <c r="N20" s="144"/>
+      <c r="O20" s="144"/>
+      <c r="P20" s="137">
+        <f>D5</f>
+        <v>1500</v>
+      </c>
+      <c r="Q20" s="143">
+        <f>J20*K20</f>
+        <v>40000</v>
+      </c>
+      <c r="R20" s="137">
+        <f>J20*L20</f>
+        <v>220</v>
+      </c>
+      <c r="S20" s="137">
+        <f>J20*P20</f>
+        <v>6000</v>
+      </c>
+      <c r="T20" s="143">
+        <f>T18-O20*K20</f>
+        <v>30000</v>
+      </c>
+      <c r="U20" s="143">
+        <f>U18-Q20</f>
+        <v>139000</v>
+      </c>
+      <c r="V20" s="143">
+        <f>V18-N20*K20</f>
+        <v>99000</v>
+      </c>
+      <c r="W20" s="137">
+        <f>W18-M20</f>
+        <v>6</v>
+      </c>
+      <c r="X20" s="137" t="b">
+        <f>IF(SUM($N$16:N21)&gt;=2*SUM($M$16:M21),TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="138"/>
+      <c r="B21" s="138"/>
+      <c r="C21" s="138"/>
+      <c r="D21" s="138"/>
+      <c r="E21" s="138"/>
+      <c r="G21" s="137"/>
+      <c r="H21" s="137"/>
+      <c r="I21" s="142"/>
+      <c r="J21" s="137"/>
+      <c r="K21" s="143"/>
+      <c r="L21" s="137"/>
+      <c r="M21" s="139"/>
+      <c r="N21" s="139"/>
+      <c r="O21" s="139"/>
+      <c r="P21" s="137"/>
+      <c r="Q21" s="143"/>
+      <c r="R21" s="137"/>
+      <c r="S21" s="137"/>
+      <c r="T21" s="137"/>
+      <c r="U21" s="137"/>
+      <c r="V21" s="137"/>
+      <c r="W21" s="137"/>
+      <c r="X21" s="137"/>
+    </row>
+    <row r="22" spans="1:24" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="138" t="s">
+        <v>153</v>
+      </c>
+      <c r="B22" s="138"/>
+      <c r="C22" s="138"/>
+      <c r="D22" s="138"/>
+      <c r="E22" s="138"/>
+      <c r="G22" s="137" t="s">
+        <v>184</v>
+      </c>
+      <c r="H22" s="137"/>
+      <c r="I22" s="142"/>
+      <c r="J22" s="137">
+        <v>20</v>
+      </c>
+      <c r="K22" s="143">
+        <f>E8</f>
+        <v>1000</v>
+      </c>
+      <c r="L22" s="137">
+        <f>C8</f>
+        <v>10</v>
+      </c>
+      <c r="M22" s="144"/>
+      <c r="N22" s="144"/>
+      <c r="O22" s="144">
+        <v>20</v>
+      </c>
+      <c r="P22" s="137">
+        <f>D8</f>
+        <v>1000</v>
+      </c>
+      <c r="Q22" s="143">
+        <f>J22*K22</f>
+        <v>20000</v>
+      </c>
+      <c r="R22" s="137">
+        <f>J22*L22</f>
+        <v>200</v>
+      </c>
+      <c r="S22" s="137">
+        <f>J22*P22</f>
+        <v>20000</v>
+      </c>
+      <c r="T22" s="143">
+        <f>T20-O22*K22</f>
+        <v>10000</v>
+      </c>
+      <c r="U22" s="143">
+        <f>U20-Q22</f>
+        <v>119000</v>
+      </c>
+      <c r="V22" s="143">
+        <f>V20-N22*K22</f>
+        <v>99000</v>
+      </c>
+      <c r="W22" s="137">
+        <f>W20-M22</f>
+        <v>6</v>
+      </c>
+      <c r="X22" s="137" t="b">
+        <f>IF(SUM($N$16:N23)&gt;=2*SUM($M$16:M23),TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="138"/>
+      <c r="B23" s="138"/>
+      <c r="C23" s="138"/>
+      <c r="D23" s="138"/>
+      <c r="E23" s="138"/>
+      <c r="G23" s="137"/>
+      <c r="H23" s="137"/>
+      <c r="I23" s="142"/>
+      <c r="J23" s="137"/>
+      <c r="K23" s="143"/>
+      <c r="L23" s="137"/>
+      <c r="M23" s="139"/>
+      <c r="N23" s="139"/>
+      <c r="O23" s="139"/>
+      <c r="P23" s="137"/>
+      <c r="Q23" s="143"/>
+      <c r="R23" s="137"/>
+      <c r="S23" s="137"/>
+      <c r="T23" s="137"/>
+      <c r="U23" s="137"/>
+      <c r="V23" s="137"/>
+      <c r="W23" s="137"/>
+      <c r="X23" s="137"/>
+    </row>
+    <row r="24" spans="1:24" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="138" t="s">
+        <v>157</v>
+      </c>
+      <c r="B24" s="138"/>
+      <c r="C24" s="138"/>
+      <c r="D24" s="138"/>
+      <c r="E24" s="138"/>
+      <c r="G24" s="137" t="s">
+        <v>183</v>
+      </c>
+      <c r="H24" s="137"/>
+      <c r="I24" s="142"/>
+      <c r="J24" s="137">
+        <v>10</v>
+      </c>
+      <c r="K24" s="143">
+        <f>E8</f>
+        <v>1000</v>
+      </c>
+      <c r="L24" s="137">
+        <f>C9</f>
+        <v>5</v>
+      </c>
+      <c r="M24" s="144"/>
+      <c r="N24" s="144"/>
+      <c r="O24" s="144">
+        <v>10</v>
+      </c>
+      <c r="P24" s="137">
+        <f>D9</f>
+        <v>800</v>
+      </c>
+      <c r="Q24" s="143">
+        <f>J24*K24</f>
+        <v>10000</v>
+      </c>
+      <c r="R24" s="137">
+        <f>J24*L24</f>
+        <v>50</v>
+      </c>
+      <c r="S24" s="137">
+        <f>J24*P24</f>
+        <v>8000</v>
+      </c>
+      <c r="T24" s="143">
+        <f>T22-O24*K24</f>
+        <v>0</v>
+      </c>
+      <c r="U24" s="143">
+        <f>U22-Q24</f>
+        <v>109000</v>
+      </c>
+      <c r="V24" s="143">
+        <f>V22-N24*K24</f>
+        <v>99000</v>
+      </c>
+      <c r="W24" s="137">
+        <f>W22-M24</f>
+        <v>6</v>
+      </c>
+      <c r="X24" s="137" t="b">
+        <f>IF(SUM($N$16:N25)&gt;=2*SUM($M$16:M25),TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="138"/>
+      <c r="B25" s="138"/>
+      <c r="C25" s="138"/>
+      <c r="D25" s="138"/>
+      <c r="E25" s="138"/>
+      <c r="G25" s="137"/>
+      <c r="H25" s="137"/>
+      <c r="I25" s="142"/>
+      <c r="J25" s="137"/>
+      <c r="K25" s="143"/>
+      <c r="L25" s="137"/>
+      <c r="M25" s="139"/>
+      <c r="N25" s="139"/>
+      <c r="O25" s="139"/>
+      <c r="P25" s="137"/>
+      <c r="Q25" s="143"/>
+      <c r="R25" s="137"/>
+      <c r="S25" s="137"/>
+      <c r="T25" s="137"/>
+      <c r="U25" s="137"/>
+      <c r="V25" s="137"/>
+      <c r="W25" s="137"/>
+      <c r="X25" s="137"/>
+    </row>
+    <row r="26" spans="1:24" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="138"/>
+      <c r="B26" s="138"/>
+      <c r="C26" s="138"/>
+      <c r="D26" s="138"/>
+      <c r="E26" s="138"/>
+      <c r="G26" s="137" t="s">
+        <v>185</v>
+      </c>
+      <c r="H26" s="137"/>
+      <c r="I26" s="142"/>
+      <c r="J26" s="137">
+        <v>15</v>
+      </c>
+      <c r="K26" s="143">
+        <f>E6</f>
+        <v>3000</v>
+      </c>
+      <c r="L26" s="137">
+        <f>C6</f>
+        <v>25</v>
+      </c>
+      <c r="M26" s="144"/>
+      <c r="N26" s="144">
+        <v>15</v>
+      </c>
+      <c r="O26" s="144"/>
+      <c r="P26" s="137">
+        <f>D6</f>
+        <v>2000</v>
+      </c>
+      <c r="Q26" s="143">
+        <f>J26*K26</f>
+        <v>45000</v>
+      </c>
+      <c r="R26" s="137">
+        <f>J26*L26</f>
+        <v>375</v>
+      </c>
+      <c r="S26" s="137">
+        <f>J26*P26</f>
+        <v>30000</v>
+      </c>
+      <c r="T26" s="143">
+        <f>T24-O26*K26</f>
+        <v>0</v>
+      </c>
+      <c r="U26" s="143">
+        <f>U24-Q26</f>
+        <v>64000</v>
+      </c>
+      <c r="V26" s="143">
+        <f>V24-N26*K26</f>
+        <v>54000</v>
+      </c>
+      <c r="W26" s="137">
+        <f>W24-M26</f>
+        <v>6</v>
+      </c>
+      <c r="X26" s="137" t="b">
+        <f>IF(SUM($N$16:N27)&gt;=2*SUM($M$16:M27),TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="138" t="s">
+        <v>154</v>
+      </c>
+      <c r="B27" s="138"/>
+      <c r="C27" s="138"/>
+      <c r="D27" s="138"/>
+      <c r="E27" s="138"/>
+      <c r="G27" s="137"/>
+      <c r="H27" s="137"/>
+      <c r="I27" s="142"/>
+      <c r="J27" s="137"/>
+      <c r="K27" s="143"/>
+      <c r="L27" s="137"/>
+      <c r="M27" s="139"/>
+      <c r="N27" s="139"/>
+      <c r="O27" s="139"/>
+      <c r="P27" s="137"/>
+      <c r="Q27" s="143"/>
+      <c r="R27" s="137"/>
+      <c r="S27" s="137"/>
+      <c r="T27" s="137"/>
+      <c r="U27" s="137"/>
+      <c r="V27" s="137"/>
+      <c r="W27" s="137"/>
+      <c r="X27" s="137"/>
+    </row>
+    <row r="28" spans="1:24" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="138"/>
+      <c r="B28" s="138"/>
+      <c r="C28" s="138"/>
+      <c r="D28" s="138"/>
+      <c r="E28" s="138"/>
+      <c r="G28" s="137" t="s">
+        <v>186</v>
+      </c>
+      <c r="H28" s="137"/>
+      <c r="I28" s="142"/>
+      <c r="J28" s="137">
+        <v>13</v>
+      </c>
+      <c r="K28" s="143">
+        <f>E6</f>
+        <v>3000</v>
+      </c>
+      <c r="L28" s="137">
+        <f>C7</f>
+        <v>20</v>
+      </c>
+      <c r="M28" s="144"/>
+      <c r="N28" s="144">
+        <v>13</v>
+      </c>
+      <c r="O28" s="144"/>
+      <c r="P28" s="137">
+        <f>D7</f>
+        <v>1200</v>
+      </c>
+      <c r="Q28" s="143">
+        <f>J28*K28</f>
+        <v>39000</v>
+      </c>
+      <c r="R28" s="137">
+        <f>J28*L28</f>
+        <v>260</v>
+      </c>
+      <c r="S28" s="137">
+        <f>J28*P28</f>
+        <v>15600</v>
+      </c>
+      <c r="T28" s="143">
+        <f>T26-O28*K28</f>
+        <v>0</v>
+      </c>
+      <c r="U28" s="143">
+        <f>U26-Q28</f>
+        <v>25000</v>
+      </c>
+      <c r="V28" s="143">
+        <f>V26-N28*K28</f>
+        <v>15000</v>
+      </c>
+      <c r="W28" s="137">
+        <f>W26-M28</f>
+        <v>6</v>
+      </c>
+      <c r="X28" s="137" t="b">
+        <f>IF(SUM($N$16:N29)&gt;=2*SUM($M$16:M29),TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A29" s="138" t="s">
+        <v>158</v>
+      </c>
+      <c r="B29" s="138"/>
+      <c r="C29" s="138"/>
+      <c r="D29" s="138"/>
+      <c r="E29" s="138"/>
+      <c r="G29" s="137"/>
+      <c r="H29" s="137"/>
+      <c r="I29" s="142"/>
+      <c r="J29" s="137"/>
+      <c r="K29" s="143"/>
+      <c r="L29" s="137"/>
+      <c r="M29" s="139"/>
+      <c r="N29" s="139"/>
+      <c r="O29" s="139"/>
+      <c r="P29" s="137"/>
+      <c r="Q29" s="143"/>
+      <c r="R29" s="137"/>
+      <c r="S29" s="137"/>
+      <c r="T29" s="137"/>
+      <c r="U29" s="137"/>
+      <c r="V29" s="137"/>
+      <c r="W29" s="137"/>
+      <c r="X29" s="137"/>
+    </row>
+    <row r="30" spans="1:24" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="138"/>
+      <c r="B30" s="138"/>
+      <c r="C30" s="138"/>
+      <c r="D30" s="138"/>
+      <c r="E30" s="138"/>
+      <c r="G30" s="159" t="s">
+        <v>187</v>
+      </c>
+      <c r="H30" s="158"/>
+      <c r="I30" s="142"/>
+      <c r="J30" s="157">
+        <f>SUM(J18:J29)</f>
+        <v>72</v>
+      </c>
+      <c r="K30" s="157"/>
+      <c r="L30" s="157"/>
+      <c r="M30" s="157">
+        <f>SUM(M16:M29)</f>
+        <v>14</v>
+      </c>
+      <c r="N30" s="157">
+        <f>SUM(N16:N29)</f>
+        <v>28</v>
+      </c>
+      <c r="O30" s="157">
+        <f>SUM(O16:O29)</f>
+        <v>30</v>
+      </c>
+      <c r="P30" s="157"/>
+      <c r="Q30" s="156">
+        <f>SUM(Q16:Q29)</f>
+        <v>254000</v>
+      </c>
+      <c r="R30" s="155">
+        <f>SUM(R16:R29)</f>
+        <v>2005</v>
+      </c>
+      <c r="S30" s="155">
+        <f>SUM(S16:S29)</f>
+        <v>119600</v>
+      </c>
+      <c r="T30" s="156">
+        <f>T28</f>
+        <v>0</v>
+      </c>
+      <c r="U30" s="156">
+        <f>U28</f>
+        <v>25000</v>
+      </c>
+      <c r="V30" s="156">
+        <f>V28</f>
+        <v>15000</v>
+      </c>
+      <c r="W30" s="155">
+        <f>W28</f>
+        <v>6</v>
+      </c>
+      <c r="X30" s="155" t="b">
+        <f>X28</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A31" s="138"/>
+      <c r="B31" s="138"/>
+      <c r="C31" s="138"/>
+      <c r="D31" s="138"/>
+      <c r="E31" s="138"/>
+      <c r="G31" s="154"/>
+      <c r="H31" s="153"/>
+      <c r="I31" s="142"/>
+      <c r="J31" s="152"/>
+      <c r="K31" s="152"/>
+      <c r="L31" s="152"/>
+      <c r="M31" s="152"/>
+      <c r="N31" s="152"/>
+      <c r="O31" s="152"/>
+      <c r="P31" s="152"/>
+      <c r="Q31" s="151"/>
+      <c r="R31" s="151"/>
+      <c r="S31" s="151"/>
+      <c r="T31" s="151"/>
+      <c r="U31" s="151"/>
+      <c r="V31" s="151"/>
+      <c r="W31" s="151"/>
+      <c r="X31" s="151"/>
+    </row>
+    <row r="32" spans="1:24" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="138" t="s">
+        <v>155</v>
+      </c>
+      <c r="B32" s="138"/>
+      <c r="C32" s="138"/>
+      <c r="D32" s="138"/>
+      <c r="E32" s="138"/>
+      <c r="G32" s="154"/>
+      <c r="H32" s="153"/>
+      <c r="I32" s="142"/>
+      <c r="J32" s="152"/>
+      <c r="K32" s="152"/>
+      <c r="L32" s="152"/>
+      <c r="M32" s="152"/>
+      <c r="N32" s="152"/>
+      <c r="O32" s="152"/>
+      <c r="P32" s="152"/>
+      <c r="Q32" s="151"/>
+      <c r="R32" s="151"/>
+      <c r="S32" s="151"/>
+      <c r="T32" s="151"/>
+      <c r="U32" s="151"/>
+      <c r="V32" s="151"/>
+      <c r="W32" s="151"/>
+      <c r="X32" s="151"/>
+    </row>
+    <row r="33" spans="1:24" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A33" s="138"/>
+      <c r="B33" s="138"/>
+      <c r="C33" s="138"/>
+      <c r="D33" s="138"/>
+      <c r="E33" s="138"/>
+      <c r="G33" s="150"/>
+      <c r="H33" s="149"/>
+      <c r="I33" s="139"/>
+      <c r="J33" s="148"/>
+      <c r="K33" s="148"/>
+      <c r="L33" s="148"/>
+      <c r="M33" s="148"/>
+      <c r="N33" s="148"/>
+      <c r="O33" s="148"/>
+      <c r="P33" s="148"/>
+      <c r="Q33" s="147"/>
+      <c r="R33" s="147"/>
+      <c r="S33" s="147"/>
+      <c r="T33" s="147"/>
+      <c r="U33" s="147"/>
+      <c r="V33" s="147"/>
+      <c r="W33" s="147"/>
+      <c r="X33" s="147"/>
+    </row>
+    <row r="34" spans="1:24" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="138" t="s">
+        <v>159</v>
+      </c>
+      <c r="B34" s="138"/>
+      <c r="C34" s="138"/>
+      <c r="D34" s="138"/>
+      <c r="E34" s="138"/>
+    </row>
+    <row r="35" spans="1:24" s="134" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="138"/>
+      <c r="B35" s="138"/>
+      <c r="C35" s="138"/>
+      <c r="D35" s="138"/>
+      <c r="E35" s="138"/>
+      <c r="G35" s="137" t="s">
+        <v>188</v>
+      </c>
+      <c r="H35" s="137"/>
+      <c r="I35" s="137"/>
+      <c r="K35" s="146" t="s">
+        <v>194</v>
+      </c>
+      <c r="L35" s="145"/>
+      <c r="M35" s="145"/>
+      <c r="N35" s="145"/>
+      <c r="O35" s="145"/>
+      <c r="P35" s="145"/>
+      <c r="Q35" s="145"/>
+      <c r="R35" s="137" t="s">
+        <v>198</v>
+      </c>
+      <c r="S35" s="137"/>
+      <c r="T35" s="137"/>
+      <c r="U35" s="137"/>
+      <c r="V35" s="137"/>
+      <c r="W35" s="137"/>
+      <c r="X35" s="137"/>
+    </row>
+    <row r="36" spans="1:24" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A36" s="138"/>
+      <c r="B36" s="138"/>
+      <c r="C36" s="138"/>
+      <c r="D36" s="138"/>
+      <c r="E36" s="138"/>
+      <c r="G36" s="137"/>
+      <c r="H36" s="137"/>
+      <c r="I36" s="137"/>
+      <c r="K36" s="146"/>
+      <c r="L36" s="145"/>
+      <c r="M36" s="145"/>
+      <c r="N36" s="145"/>
+      <c r="O36" s="145"/>
+      <c r="P36" s="145"/>
+      <c r="Q36" s="145"/>
+      <c r="R36" s="144"/>
+      <c r="S36" s="141" t="s">
+        <v>182</v>
+      </c>
+      <c r="T36" s="141" t="s">
+        <v>196</v>
+      </c>
+      <c r="U36" s="141" t="s">
+        <v>195</v>
+      </c>
+      <c r="V36" s="141" t="s">
+        <v>205</v>
+      </c>
+      <c r="W36" s="141" t="s">
+        <v>206</v>
+      </c>
+      <c r="X36" s="144"/>
+    </row>
+    <row r="37" spans="1:24" s="134" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="138" t="s">
         <v>160</v>
       </c>
-      <c r="B14" s="135"/>
-      <c r="C14" s="135"/>
-      <c r="D14" s="135"/>
-      <c r="E14" s="135"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="135"/>
-      <c r="B15" s="135"/>
-      <c r="C15" s="135"/>
-      <c r="D15" s="135"/>
-      <c r="E15" s="135"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="135"/>
-      <c r="B16" s="135"/>
-      <c r="C16" s="135"/>
-      <c r="D16" s="135"/>
-      <c r="E16" s="135"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="132" t="s">
-        <v>152</v>
-      </c>
-      <c r="B17" s="133"/>
-      <c r="C17" s="133"/>
-      <c r="D17" s="133"/>
-      <c r="E17" s="133"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="133"/>
-      <c r="B18" s="133"/>
-      <c r="C18" s="133"/>
-      <c r="D18" s="133"/>
-      <c r="E18" s="133"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="132" t="s">
-        <v>156</v>
-      </c>
-      <c r="B19" s="133"/>
-      <c r="C19" s="133"/>
-      <c r="D19" s="133"/>
-      <c r="E19" s="133"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="133"/>
-      <c r="B20" s="133"/>
-      <c r="C20" s="133"/>
-      <c r="D20" s="133"/>
-      <c r="E20" s="133"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="133"/>
-      <c r="B21" s="133"/>
-      <c r="C21" s="133"/>
-      <c r="D21" s="133"/>
-      <c r="E21" s="133"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="132" t="s">
-        <v>153</v>
-      </c>
-      <c r="B22" s="133"/>
-      <c r="C22" s="133"/>
-      <c r="D22" s="133"/>
-      <c r="E22" s="133"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="133"/>
-      <c r="B23" s="133"/>
-      <c r="C23" s="133"/>
-      <c r="D23" s="133"/>
-      <c r="E23" s="133"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="132" t="s">
-        <v>157</v>
-      </c>
-      <c r="B24" s="133"/>
-      <c r="C24" s="133"/>
-      <c r="D24" s="133"/>
-      <c r="E24" s="133"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="133"/>
-      <c r="B25" s="133"/>
-      <c r="C25" s="133"/>
-      <c r="D25" s="133"/>
-      <c r="E25" s="133"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="133"/>
-      <c r="B26" s="133"/>
-      <c r="C26" s="133"/>
-      <c r="D26" s="133"/>
-      <c r="E26" s="133"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="132" t="s">
-        <v>154</v>
-      </c>
-      <c r="B27" s="133"/>
-      <c r="C27" s="133"/>
-      <c r="D27" s="133"/>
-      <c r="E27" s="133"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="133"/>
-      <c r="B28" s="133"/>
-      <c r="C28" s="133"/>
-      <c r="D28" s="133"/>
-      <c r="E28" s="133"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="132" t="s">
-        <v>158</v>
-      </c>
-      <c r="B29" s="133"/>
-      <c r="C29" s="133"/>
-      <c r="D29" s="133"/>
-      <c r="E29" s="133"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="133"/>
-      <c r="B30" s="133"/>
-      <c r="C30" s="133"/>
-      <c r="D30" s="133"/>
-      <c r="E30" s="133"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="133"/>
-      <c r="B31" s="133"/>
-      <c r="C31" s="133"/>
-      <c r="D31" s="133"/>
-      <c r="E31" s="133"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="132" t="s">
-        <v>155</v>
-      </c>
-      <c r="B32" s="133"/>
-      <c r="C32" s="133"/>
-      <c r="D32" s="133"/>
-      <c r="E32" s="133"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="133"/>
-      <c r="B33" s="133"/>
-      <c r="C33" s="133"/>
-      <c r="D33" s="133"/>
-      <c r="E33" s="133"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="132" t="s">
-        <v>159</v>
-      </c>
-      <c r="B34" s="133"/>
-      <c r="C34" s="133"/>
-      <c r="D34" s="133"/>
-      <c r="E34" s="133"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="133"/>
-      <c r="B35" s="133"/>
-      <c r="C35" s="133"/>
-      <c r="D35" s="133"/>
-      <c r="E35" s="133"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="133"/>
-      <c r="B36" s="133"/>
-      <c r="C36" s="133"/>
-      <c r="D36" s="133"/>
-      <c r="E36" s="133"/>
-    </row>
-    <row r="37" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048550" spans="16384:16384" x14ac:dyDescent="0.2">
-      <c r="XFD1048550">
+      <c r="B37" s="138"/>
+      <c r="C37" s="138"/>
+      <c r="D37" s="138"/>
+      <c r="E37" s="138"/>
+      <c r="G37" s="137" t="s">
+        <v>174</v>
+      </c>
+      <c r="H37" s="143">
+        <f>U30</f>
+        <v>25000</v>
+      </c>
+      <c r="I37" s="137"/>
+      <c r="K37" s="136" t="s">
+        <v>197</v>
+      </c>
+      <c r="L37" s="136"/>
+      <c r="M37" s="136"/>
+      <c r="N37" s="136"/>
+      <c r="O37" s="136"/>
+      <c r="P37" s="136"/>
+      <c r="Q37" s="136"/>
+      <c r="R37" s="142"/>
+      <c r="S37" s="141">
+        <v>0</v>
+      </c>
+      <c r="T37" s="141">
+        <v>0</v>
+      </c>
+      <c r="U37" s="141">
+        <v>9</v>
+      </c>
+      <c r="V37" s="141">
+        <f>$R$30</f>
+        <v>2005</v>
+      </c>
+      <c r="W37" s="141">
+        <f>55*S37+20*T37+5*U37+V37</f>
+        <v>2050</v>
+      </c>
+      <c r="X37" s="142"/>
+    </row>
+    <row r="38" spans="1:24" s="134" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="138"/>
+      <c r="B38" s="138"/>
+      <c r="C38" s="138"/>
+      <c r="D38" s="138"/>
+      <c r="E38" s="138"/>
+      <c r="G38" s="137"/>
+      <c r="H38" s="137"/>
+      <c r="I38" s="137"/>
+      <c r="K38" s="136"/>
+      <c r="L38" s="136"/>
+      <c r="M38" s="136"/>
+      <c r="N38" s="136"/>
+      <c r="O38" s="136"/>
+      <c r="P38" s="136"/>
+      <c r="Q38" s="136"/>
+      <c r="R38" s="142"/>
+      <c r="S38" s="141">
+        <v>0</v>
+      </c>
+      <c r="T38" s="141">
+        <v>5</v>
+      </c>
+      <c r="U38" s="141">
+        <v>0</v>
+      </c>
+      <c r="V38" s="141">
+        <f>$R$30</f>
+        <v>2005</v>
+      </c>
+      <c r="W38" s="141">
+        <f>55*S38+20*T38+5*U38+V38</f>
+        <v>2105</v>
+      </c>
+      <c r="X38" s="142"/>
+    </row>
+    <row r="39" spans="1:24" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A39" s="138" t="s">
+        <v>161</v>
+      </c>
+      <c r="B39" s="138"/>
+      <c r="C39" s="138"/>
+      <c r="D39" s="138"/>
+      <c r="E39" s="138"/>
+      <c r="G39" s="137" t="s">
+        <v>189</v>
+      </c>
+      <c r="H39" s="137">
+        <f>M30</f>
+        <v>14</v>
+      </c>
+      <c r="I39" s="137"/>
+      <c r="K39" s="136"/>
+      <c r="L39" s="136"/>
+      <c r="M39" s="136"/>
+      <c r="N39" s="136"/>
+      <c r="O39" s="136"/>
+      <c r="P39" s="136"/>
+      <c r="Q39" s="136"/>
+      <c r="R39" s="142"/>
+      <c r="S39" s="141">
+        <v>1</v>
+      </c>
+      <c r="T39" s="141">
+        <v>0</v>
+      </c>
+      <c r="U39" s="141">
+        <v>9</v>
+      </c>
+      <c r="V39" s="141">
+        <f>$R$30</f>
+        <v>2005</v>
+      </c>
+      <c r="W39" s="141">
+        <f>55*S39+20*T39+5*U39+V39</f>
+        <v>2105</v>
+      </c>
+      <c r="X39" s="142"/>
+    </row>
+    <row r="40" spans="1:24" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A40" s="138"/>
+      <c r="B40" s="138"/>
+      <c r="C40" s="138"/>
+      <c r="D40" s="138"/>
+      <c r="E40" s="138"/>
+      <c r="G40" s="137"/>
+      <c r="H40" s="137"/>
+      <c r="I40" s="137"/>
+      <c r="K40" s="136"/>
+      <c r="L40" s="136"/>
+      <c r="M40" s="136"/>
+      <c r="N40" s="136"/>
+      <c r="O40" s="136"/>
+      <c r="P40" s="136"/>
+      <c r="Q40" s="136"/>
+      <c r="R40" s="139"/>
+      <c r="S40" s="141">
+        <v>1</v>
+      </c>
+      <c r="T40" s="141">
+        <v>5</v>
+      </c>
+      <c r="U40" s="141">
+        <v>0</v>
+      </c>
+      <c r="V40" s="141">
+        <f>$R$30</f>
+        <v>2005</v>
+      </c>
+      <c r="W40" s="140">
+        <f>55*S40+20*T40+5*U40+V40</f>
+        <v>2160</v>
+      </c>
+      <c r="X40" s="139"/>
+    </row>
+    <row r="41" spans="1:24" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A41" s="138"/>
+      <c r="B41" s="138"/>
+      <c r="C41" s="138"/>
+      <c r="D41" s="138"/>
+      <c r="E41" s="138"/>
+      <c r="G41" s="137" t="s">
+        <v>191</v>
+      </c>
+      <c r="H41" s="137">
+        <f>N30</f>
+        <v>28</v>
+      </c>
+      <c r="I41" s="137"/>
+      <c r="K41" s="136"/>
+      <c r="L41" s="136"/>
+      <c r="M41" s="136"/>
+      <c r="N41" s="136"/>
+      <c r="O41" s="136"/>
+      <c r="P41" s="136"/>
+      <c r="Q41" s="136"/>
+    </row>
+    <row r="42" spans="1:24" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A42" s="138" t="s">
+        <v>162</v>
+      </c>
+      <c r="B42" s="138"/>
+      <c r="C42" s="138"/>
+      <c r="D42" s="138"/>
+      <c r="E42" s="138"/>
+      <c r="G42" s="137"/>
+      <c r="H42" s="137"/>
+      <c r="I42" s="137"/>
+      <c r="K42" s="136"/>
+      <c r="L42" s="136"/>
+      <c r="M42" s="136"/>
+      <c r="N42" s="136"/>
+      <c r="O42" s="136"/>
+      <c r="P42" s="136"/>
+      <c r="Q42" s="136"/>
+    </row>
+    <row r="43" spans="1:24" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A43" s="138"/>
+      <c r="B43" s="138"/>
+      <c r="C43" s="138"/>
+      <c r="D43" s="138"/>
+      <c r="E43" s="138"/>
+      <c r="G43" s="137" t="s">
+        <v>190</v>
+      </c>
+      <c r="H43" s="137">
+        <f>O30</f>
+        <v>30</v>
+      </c>
+      <c r="I43" s="137"/>
+      <c r="K43" s="136"/>
+      <c r="L43" s="136"/>
+      <c r="M43" s="136"/>
+      <c r="N43" s="136"/>
+      <c r="O43" s="136"/>
+      <c r="P43" s="136"/>
+      <c r="Q43" s="136"/>
+    </row>
+    <row r="44" spans="1:24" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A44" s="138" t="s">
+        <v>163</v>
+      </c>
+      <c r="B44" s="138"/>
+      <c r="C44" s="138"/>
+      <c r="D44" s="138"/>
+      <c r="E44" s="138"/>
+      <c r="G44" s="137"/>
+      <c r="H44" s="137"/>
+      <c r="I44" s="137"/>
+      <c r="K44" s="136"/>
+      <c r="L44" s="136"/>
+      <c r="M44" s="136"/>
+      <c r="N44" s="136"/>
+      <c r="O44" s="136"/>
+      <c r="P44" s="136"/>
+      <c r="Q44" s="136"/>
+    </row>
+    <row r="45" spans="1:24" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A45" s="138"/>
+      <c r="B45" s="138"/>
+      <c r="C45" s="138"/>
+      <c r="D45" s="138"/>
+      <c r="E45" s="138"/>
+      <c r="G45" s="137" t="s">
+        <v>192</v>
+      </c>
+      <c r="H45" s="137">
+        <f>W30</f>
+        <v>6</v>
+      </c>
+      <c r="I45" s="137"/>
+      <c r="K45" s="136"/>
+      <c r="L45" s="136"/>
+      <c r="M45" s="136"/>
+      <c r="N45" s="136"/>
+      <c r="O45" s="136"/>
+      <c r="P45" s="136"/>
+      <c r="Q45" s="136"/>
+    </row>
+    <row r="46" spans="1:24" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A46" s="138"/>
+      <c r="B46" s="138"/>
+      <c r="C46" s="138"/>
+      <c r="D46" s="138"/>
+      <c r="E46" s="138"/>
+      <c r="G46" s="137"/>
+      <c r="H46" s="137"/>
+      <c r="I46" s="137"/>
+      <c r="K46" s="136"/>
+      <c r="L46" s="136"/>
+      <c r="M46" s="136"/>
+      <c r="N46" s="136"/>
+      <c r="O46" s="136"/>
+      <c r="P46" s="136"/>
+      <c r="Q46" s="136"/>
+    </row>
+    <row r="47" spans="1:24" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="G47" s="137" t="s">
+        <v>193</v>
+      </c>
+      <c r="H47" s="137">
+        <f>V30/E8</f>
+        <v>15</v>
+      </c>
+      <c r="I47" s="137"/>
+      <c r="K47" s="136"/>
+      <c r="L47" s="136"/>
+      <c r="M47" s="136"/>
+      <c r="N47" s="136"/>
+      <c r="O47" s="136"/>
+      <c r="P47" s="136"/>
+      <c r="Q47" s="136"/>
+    </row>
+    <row r="48" spans="1:24" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="G48" s="137"/>
+      <c r="H48" s="137"/>
+      <c r="I48" s="137"/>
+      <c r="K48" s="136"/>
+      <c r="L48" s="136"/>
+      <c r="M48" s="136"/>
+      <c r="N48" s="136"/>
+      <c r="O48" s="136"/>
+      <c r="P48" s="136"/>
+      <c r="Q48" s="136"/>
+    </row>
+    <row r="49" spans="11:17" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K49" s="136"/>
+      <c r="L49" s="136"/>
+      <c r="M49" s="136"/>
+      <c r="N49" s="136"/>
+      <c r="O49" s="136"/>
+      <c r="P49" s="136"/>
+      <c r="Q49" s="136"/>
+    </row>
+    <row r="50" spans="11:17" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K50" s="136"/>
+      <c r="L50" s="136"/>
+      <c r="M50" s="136"/>
+      <c r="N50" s="136"/>
+      <c r="O50" s="136"/>
+      <c r="P50" s="136"/>
+      <c r="Q50" s="136"/>
+    </row>
+    <row r="51" spans="11:17" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K51" s="136"/>
+      <c r="L51" s="136"/>
+      <c r="M51" s="136"/>
+      <c r="N51" s="136"/>
+      <c r="O51" s="136"/>
+      <c r="P51" s="136"/>
+      <c r="Q51" s="136"/>
+    </row>
+    <row r="52" spans="11:17" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K52" s="136"/>
+      <c r="L52" s="136"/>
+      <c r="M52" s="136"/>
+      <c r="N52" s="136"/>
+      <c r="O52" s="136"/>
+      <c r="P52" s="136"/>
+      <c r="Q52" s="136"/>
+    </row>
+    <row r="53" spans="11:17" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K53" s="136"/>
+      <c r="L53" s="136"/>
+      <c r="M53" s="136"/>
+      <c r="N53" s="136"/>
+      <c r="O53" s="136"/>
+      <c r="P53" s="136"/>
+      <c r="Q53" s="136"/>
+    </row>
+    <row r="54" spans="11:17" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K54" s="136"/>
+      <c r="L54" s="136"/>
+      <c r="M54" s="136"/>
+      <c r="N54" s="136"/>
+      <c r="O54" s="136"/>
+      <c r="P54" s="136"/>
+      <c r="Q54" s="136"/>
+    </row>
+    <row r="55" spans="11:17" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K55" s="136"/>
+      <c r="L55" s="136"/>
+      <c r="M55" s="136"/>
+      <c r="N55" s="136"/>
+      <c r="O55" s="136"/>
+      <c r="P55" s="136"/>
+      <c r="Q55" s="136"/>
+    </row>
+    <row r="56" spans="11:17" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K56" s="136"/>
+      <c r="L56" s="136"/>
+      <c r="M56" s="136"/>
+      <c r="N56" s="136"/>
+      <c r="O56" s="136"/>
+      <c r="P56" s="136"/>
+      <c r="Q56" s="136"/>
+    </row>
+    <row r="57" spans="11:17" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K57" s="136"/>
+      <c r="L57" s="136"/>
+      <c r="M57" s="136"/>
+      <c r="N57" s="136"/>
+      <c r="O57" s="136"/>
+      <c r="P57" s="136"/>
+      <c r="Q57" s="136"/>
+    </row>
+    <row r="58" spans="11:17" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K58" s="136"/>
+      <c r="L58" s="136"/>
+      <c r="M58" s="136"/>
+      <c r="N58" s="136"/>
+      <c r="O58" s="136"/>
+      <c r="P58" s="136"/>
+      <c r="Q58" s="136"/>
+    </row>
+    <row r="59" spans="11:17" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K59" s="136"/>
+      <c r="L59" s="136"/>
+      <c r="M59" s="136"/>
+      <c r="N59" s="136"/>
+      <c r="O59" s="136"/>
+      <c r="P59" s="136"/>
+      <c r="Q59" s="136"/>
+    </row>
+    <row r="60" spans="11:17" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K60" s="136"/>
+      <c r="L60" s="136"/>
+      <c r="M60" s="136"/>
+      <c r="N60" s="136"/>
+      <c r="O60" s="136"/>
+      <c r="P60" s="136"/>
+      <c r="Q60" s="136"/>
+    </row>
+    <row r="61" spans="11:17" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K61" s="136"/>
+      <c r="L61" s="136"/>
+      <c r="M61" s="136"/>
+      <c r="N61" s="136"/>
+      <c r="O61" s="136"/>
+      <c r="P61" s="136"/>
+      <c r="Q61" s="136"/>
+    </row>
+    <row r="62" spans="11:17" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K62" s="136"/>
+      <c r="L62" s="136"/>
+      <c r="M62" s="136"/>
+      <c r="N62" s="136"/>
+      <c r="O62" s="136"/>
+      <c r="P62" s="136"/>
+      <c r="Q62" s="136"/>
+    </row>
+    <row r="63" spans="11:17" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K63" s="136"/>
+      <c r="L63" s="136"/>
+      <c r="M63" s="136"/>
+      <c r="N63" s="136"/>
+      <c r="O63" s="136"/>
+      <c r="P63" s="136"/>
+      <c r="Q63" s="136"/>
+    </row>
+    <row r="64" spans="11:17" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K64" s="136"/>
+      <c r="L64" s="136"/>
+      <c r="M64" s="136"/>
+      <c r="N64" s="136"/>
+      <c r="O64" s="136"/>
+      <c r="P64" s="136"/>
+      <c r="Q64" s="136"/>
+    </row>
+    <row r="65" spans="11:17" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K65" s="136"/>
+      <c r="L65" s="136"/>
+      <c r="M65" s="136"/>
+      <c r="N65" s="136"/>
+      <c r="O65" s="136"/>
+      <c r="P65" s="136"/>
+      <c r="Q65" s="136"/>
+    </row>
+    <row r="66" spans="11:17" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K66" s="136"/>
+      <c r="L66" s="136"/>
+      <c r="M66" s="136"/>
+      <c r="N66" s="136"/>
+      <c r="O66" s="136"/>
+      <c r="P66" s="136"/>
+      <c r="Q66" s="136"/>
+    </row>
+    <row r="67" spans="11:17" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K67" s="136"/>
+      <c r="L67" s="136"/>
+      <c r="M67" s="136"/>
+      <c r="N67" s="136"/>
+      <c r="O67" s="136"/>
+      <c r="P67" s="136"/>
+      <c r="Q67" s="136"/>
+    </row>
+    <row r="68" spans="11:17" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K68" s="136"/>
+      <c r="L68" s="136"/>
+      <c r="M68" s="136"/>
+      <c r="N68" s="136"/>
+      <c r="O68" s="136"/>
+      <c r="P68" s="136"/>
+      <c r="Q68" s="136"/>
+    </row>
+    <row r="69" spans="11:17" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K69" s="136"/>
+      <c r="L69" s="136"/>
+      <c r="M69" s="136"/>
+      <c r="N69" s="136"/>
+      <c r="O69" s="136"/>
+      <c r="P69" s="136"/>
+      <c r="Q69" s="136"/>
+    </row>
+    <row r="70" spans="11:17" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K70" s="136"/>
+      <c r="L70" s="136"/>
+      <c r="M70" s="136"/>
+      <c r="N70" s="136"/>
+      <c r="O70" s="136"/>
+      <c r="P70" s="136"/>
+      <c r="Q70" s="136"/>
+    </row>
+    <row r="71" spans="11:17" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K71" s="136"/>
+      <c r="L71" s="136"/>
+      <c r="M71" s="136"/>
+      <c r="N71" s="136"/>
+      <c r="O71" s="136"/>
+      <c r="P71" s="136"/>
+      <c r="Q71" s="136"/>
+    </row>
+    <row r="72" spans="11:17" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K72" s="136"/>
+      <c r="L72" s="136"/>
+      <c r="M72" s="136"/>
+      <c r="N72" s="136"/>
+      <c r="O72" s="136"/>
+      <c r="P72" s="136"/>
+      <c r="Q72" s="136"/>
+    </row>
+    <row r="73" spans="11:17" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K73" s="136"/>
+      <c r="L73" s="136"/>
+      <c r="M73" s="136"/>
+      <c r="N73" s="136"/>
+      <c r="O73" s="136"/>
+      <c r="P73" s="136"/>
+      <c r="Q73" s="136"/>
+    </row>
+    <row r="74" spans="11:17" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K74" s="136"/>
+      <c r="L74" s="136"/>
+      <c r="M74" s="136"/>
+      <c r="N74" s="136"/>
+      <c r="O74" s="136"/>
+      <c r="P74" s="136"/>
+      <c r="Q74" s="136"/>
+    </row>
+    <row r="1048550" spans="12618:12618" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="RQH1048550" s="134">
         <f>solver_pre</f>
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="1048551" spans="16384:16384" x14ac:dyDescent="0.2">
-      <c r="XFD1048551">
+    <row r="1048551" spans="12618:12618" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="RQH1048551" s="134">
         <f>solver_scl</f>
         <v>2</v>
       </c>
     </row>
-    <row r="1048552" spans="16384:16384" x14ac:dyDescent="0.2">
-      <c r="XFD1048552">
+    <row r="1048552" spans="12618:12618" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="RQH1048552" s="134">
         <f>solver_rlx</f>
         <v>2</v>
       </c>
     </row>
-    <row r="1048553" spans="16384:16384" x14ac:dyDescent="0.2">
-      <c r="XFD1048553">
+    <row r="1048553" spans="12618:12618" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="RQH1048553" s="134">
         <f>solver_tol</f>
         <v>0.01</v>
       </c>
     </row>
-    <row r="1048554" spans="16384:16384" x14ac:dyDescent="0.2">
-      <c r="XFD1048554">
+    <row r="1048554" spans="12618:12618" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="RQH1048554" s="134">
         <f>solver_cvg</f>
         <v>1E-4</v>
       </c>
     </row>
-    <row r="1048555" spans="16384:16384" x14ac:dyDescent="0.2">
-      <c r="XFD1048555" t="e" cm="1">
-        <f t="array" ref="XFD1048555">AREAS(solver_adj1)</f>
+    <row r="1048555" spans="12618:12618" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="RQH1048555" s="134" t="e" cm="1">
+        <f t="array" ref="RQH1048555">AREAS(solver_adj1)</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="1048556" spans="16384:16384" x14ac:dyDescent="0.2">
-      <c r="XFD1048556">
+    <row r="1048556" spans="12618:12618" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="RQH1048556" s="134">
         <f>solver_ssz</f>
         <v>100</v>
       </c>
     </row>
-    <row r="1048557" spans="16384:16384" x14ac:dyDescent="0.2">
-      <c r="XFD1048557">
+    <row r="1048557" spans="12618:12618" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="RQH1048557" s="134">
         <f>solver_rsd</f>
         <v>0</v>
       </c>
     </row>
-    <row r="1048558" spans="16384:16384" x14ac:dyDescent="0.2">
-      <c r="XFD1048558">
+    <row r="1048558" spans="12618:12618" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="RQH1048558" s="134">
         <f>solver_mrt</f>
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="1048559" spans="16384:16384" x14ac:dyDescent="0.2">
-      <c r="XFD1048559">
+    <row r="1048559" spans="12618:12618" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="RQH1048559" s="134">
         <f>solver_mni</f>
         <v>30</v>
       </c>
     </row>
-    <row r="1048560" spans="16384:16384" x14ac:dyDescent="0.2">
-      <c r="XFD1048560">
+    <row r="1048560" spans="12618:12618" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="RQH1048560" s="134">
         <f>solver_rbv</f>
         <v>2</v>
       </c>
     </row>
-    <row r="1048561" spans="16384:16384" x14ac:dyDescent="0.2">
-      <c r="XFD1048561">
+    <row r="1048561" spans="12618:12618" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="RQH1048561" s="134">
         <f>solver_neg</f>
         <v>2</v>
       </c>
     </row>
-    <row r="1048562" spans="16384:16384" x14ac:dyDescent="0.2">
-      <c r="XFD1048562" t="e" cm="1">
-        <f t="array" ref="XFD1048562">solver_ntr</f>
+    <row r="1048562" spans="12618:12618" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="RQH1048562" s="134" t="e" cm="1">
+        <f t="array" ref="RQH1048562">solver_ntr</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="1048563" spans="16384:16384" x14ac:dyDescent="0.2">
-      <c r="XFD1048563" t="e" cm="1">
-        <f t="array" ref="XFD1048563">solver_acc</f>
+    <row r="1048563" spans="12618:12618" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="RQH1048563" s="134" t="e" cm="1">
+        <f t="array" ref="RQH1048563">solver_acc</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="1048564" spans="16384:16384" x14ac:dyDescent="0.2">
-      <c r="XFD1048564" t="e" cm="1">
-        <f t="array" ref="XFD1048564">solver_res</f>
+    <row r="1048564" spans="12618:12618" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="RQH1048564" s="134" t="e" cm="1">
+        <f t="array" ref="RQH1048564">solver_res</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="1048565" spans="16384:16384" x14ac:dyDescent="0.2">
-      <c r="XFD1048565" t="e" cm="1">
-        <f t="array" ref="XFD1048565">solver_ars</f>
+    <row r="1048565" spans="12618:12618" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="RQH1048565" s="134" t="e" cm="1">
+        <f t="array" ref="RQH1048565">solver_ars</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="1048566" spans="16384:16384" x14ac:dyDescent="0.2">
-      <c r="XFD1048566" t="e" cm="1">
-        <f t="array" ref="XFD1048566">solver_sta</f>
+    <row r="1048566" spans="12618:12618" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="RQH1048566" s="134" t="e" cm="1">
+        <f t="array" ref="RQH1048566">solver_sta</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="1048567" spans="16384:16384" x14ac:dyDescent="0.2">
-      <c r="XFD1048567" t="e" cm="1">
-        <f t="array" ref="XFD1048567">solver_met</f>
+    <row r="1048567" spans="12618:12618" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="RQH1048567" s="134" t="e" cm="1">
+        <f t="array" ref="RQH1048567">solver_met</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="1048568" spans="16384:16384" x14ac:dyDescent="0.2">
-      <c r="XFD1048568" t="e" cm="1">
-        <f t="array" ref="XFD1048568">solver_soc</f>
+    <row r="1048568" spans="12618:12618" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="RQH1048568" s="134" t="e" cm="1">
+        <f t="array" ref="RQH1048568">solver_soc</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="1048569" spans="16384:16384" x14ac:dyDescent="0.2">
-      <c r="XFD1048569" t="e" cm="1">
-        <f t="array" ref="XFD1048569">solver_lpt</f>
+    <row r="1048569" spans="12618:12618" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="RQH1048569" s="134" t="e" cm="1">
+        <f t="array" ref="RQH1048569">solver_lpt</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="1048570" spans="16384:16384" x14ac:dyDescent="0.2">
-      <c r="XFD1048570" t="e" cm="1">
-        <f t="array" ref="XFD1048570">solver_lpp</f>
+    <row r="1048570" spans="12618:12618" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="RQH1048570" s="134" t="e" cm="1">
+        <f t="array" ref="RQH1048570">solver_lpp</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="1048571" spans="16384:16384" x14ac:dyDescent="0.2">
-      <c r="XFD1048571" t="e" cm="1">
-        <f t="array" ref="XFD1048571">solver_gap</f>
+    <row r="1048571" spans="12618:12618" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="RQH1048571" s="134" t="e" cm="1">
+        <f t="array" ref="RQH1048571">solver_gap</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="1048572" spans="16384:16384" x14ac:dyDescent="0.2">
-      <c r="XFD1048572" t="e" cm="1">
-        <f t="array" ref="XFD1048572">solver_ips</f>
+    <row r="1048572" spans="12618:12618" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="RQH1048572" s="134" t="e" cm="1">
+        <f t="array" ref="RQH1048572">solver_ips</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="1048573" spans="16384:16384" x14ac:dyDescent="0.2">
-      <c r="XFD1048573" t="e" cm="1">
-        <f t="array" ref="XFD1048573">solver_fea</f>
+    <row r="1048573" spans="12618:12618" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="RQH1048573" s="134" t="e" cm="1">
+        <f t="array" ref="RQH1048573">solver_fea</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="1048574" spans="16384:16384" x14ac:dyDescent="0.2">
-      <c r="XFD1048574" t="e" cm="1">
-        <f t="array" ref="XFD1048574">solver_ipi</f>
+    <row r="1048574" spans="12618:12618" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="RQH1048574" s="134" t="e" cm="1">
+        <f t="array" ref="RQH1048574">solver_ipi</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="1048575" spans="16384:16384" x14ac:dyDescent="0.2">
-      <c r="XFD1048575" t="e" cm="1">
-        <f t="array" ref="XFD1048575">solver_ipd</f>
+    <row r="1048575" spans="12618:12618" s="134" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="RQH1048575" s="134" t="e" cm="1">
+        <f t="array" ref="RQH1048575">solver_ipd</f>
         <v>#NAME?</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="193">
+    <mergeCell ref="A1:S2"/>
+    <mergeCell ref="A12:B13"/>
+    <mergeCell ref="C12:E13"/>
+    <mergeCell ref="A14:E16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="C17:E18"/>
     <mergeCell ref="A29:E31"/>
     <mergeCell ref="A32:B33"/>
     <mergeCell ref="C32:E33"/>
@@ -10431,11 +12565,829 @@
     <mergeCell ref="A24:E26"/>
     <mergeCell ref="A27:B28"/>
     <mergeCell ref="C27:E28"/>
-    <mergeCell ref="A12:B13"/>
-    <mergeCell ref="C12:E13"/>
-    <mergeCell ref="A14:E16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="C17:E18"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A44:E46"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="C37:E38"/>
+    <mergeCell ref="A39:E41"/>
+    <mergeCell ref="A42:B43"/>
+    <mergeCell ref="C42:E43"/>
+    <mergeCell ref="L20:L21"/>
+    <mergeCell ref="P20:P21"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="N24:N25"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="R20:R21"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="M20:M21"/>
+    <mergeCell ref="N20:N21"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="O20:O21"/>
+    <mergeCell ref="P14:P15"/>
+    <mergeCell ref="Q14:Q15"/>
+    <mergeCell ref="R14:R15"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="P16:P17"/>
+    <mergeCell ref="Q16:Q17"/>
+    <mergeCell ref="R16:R17"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="P22:P23"/>
+    <mergeCell ref="Q22:Q23"/>
+    <mergeCell ref="R22:R23"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="P24:P25"/>
+    <mergeCell ref="Q24:Q25"/>
+    <mergeCell ref="R24:R25"/>
+    <mergeCell ref="Q18:Q19"/>
+    <mergeCell ref="P26:P27"/>
+    <mergeCell ref="Q26:Q27"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="J28:J29"/>
+    <mergeCell ref="K28:K29"/>
+    <mergeCell ref="L28:L29"/>
+    <mergeCell ref="P28:P29"/>
+    <mergeCell ref="Q28:Q29"/>
+    <mergeCell ref="R28:R29"/>
+    <mergeCell ref="S14:S15"/>
+    <mergeCell ref="T14:T15"/>
+    <mergeCell ref="S16:S17"/>
+    <mergeCell ref="T16:T17"/>
+    <mergeCell ref="S18:S19"/>
+    <mergeCell ref="T18:T19"/>
+    <mergeCell ref="G14:H15"/>
+    <mergeCell ref="G16:H17"/>
+    <mergeCell ref="G18:H19"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="P18:P19"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="S26:S27"/>
+    <mergeCell ref="T26:T27"/>
+    <mergeCell ref="S28:S29"/>
+    <mergeCell ref="T28:T29"/>
+    <mergeCell ref="S20:S21"/>
+    <mergeCell ref="T20:T21"/>
+    <mergeCell ref="S22:S23"/>
+    <mergeCell ref="T22:T23"/>
+    <mergeCell ref="S24:S25"/>
+    <mergeCell ref="T24:T25"/>
+    <mergeCell ref="V24:V25"/>
+    <mergeCell ref="V26:V27"/>
+    <mergeCell ref="V28:V29"/>
+    <mergeCell ref="V14:V15"/>
+    <mergeCell ref="V16:V17"/>
+    <mergeCell ref="V18:V19"/>
+    <mergeCell ref="V20:V21"/>
+    <mergeCell ref="V22:V23"/>
+    <mergeCell ref="U14:U15"/>
+    <mergeCell ref="U16:U17"/>
+    <mergeCell ref="U18:U19"/>
+    <mergeCell ref="U20:U21"/>
+    <mergeCell ref="U22:U23"/>
+    <mergeCell ref="U24:U25"/>
+    <mergeCell ref="U26:U27"/>
+    <mergeCell ref="U28:U29"/>
+    <mergeCell ref="X24:X25"/>
+    <mergeCell ref="X26:X27"/>
+    <mergeCell ref="X28:X29"/>
+    <mergeCell ref="X14:X15"/>
+    <mergeCell ref="X16:X17"/>
+    <mergeCell ref="X18:X19"/>
+    <mergeCell ref="X20:X21"/>
+    <mergeCell ref="X22:X23"/>
+    <mergeCell ref="W14:W15"/>
+    <mergeCell ref="W16:W17"/>
+    <mergeCell ref="W18:W19"/>
+    <mergeCell ref="W20:W21"/>
+    <mergeCell ref="W22:W23"/>
+    <mergeCell ref="W24:W25"/>
+    <mergeCell ref="W26:W27"/>
+    <mergeCell ref="W28:W29"/>
+    <mergeCell ref="G30:H33"/>
+    <mergeCell ref="I14:I33"/>
+    <mergeCell ref="J30:J33"/>
+    <mergeCell ref="K30:K33"/>
+    <mergeCell ref="L30:L33"/>
+    <mergeCell ref="O14:O15"/>
+    <mergeCell ref="O16:O17"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="O22:O23"/>
+    <mergeCell ref="O24:O25"/>
+    <mergeCell ref="O26:O27"/>
+    <mergeCell ref="O28:O29"/>
+    <mergeCell ref="G20:H21"/>
+    <mergeCell ref="G22:H23"/>
+    <mergeCell ref="G24:H25"/>
+    <mergeCell ref="G26:H27"/>
+    <mergeCell ref="G28:H29"/>
+    <mergeCell ref="N26:N27"/>
+    <mergeCell ref="M30:M33"/>
+    <mergeCell ref="N30:N33"/>
+    <mergeCell ref="L26:L27"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="K20:K21"/>
+    <mergeCell ref="M28:M29"/>
+    <mergeCell ref="N28:N29"/>
+    <mergeCell ref="M26:M27"/>
+    <mergeCell ref="U30:U33"/>
+    <mergeCell ref="V30:V33"/>
+    <mergeCell ref="W30:W33"/>
+    <mergeCell ref="X30:X33"/>
+    <mergeCell ref="O30:O33"/>
+    <mergeCell ref="P30:P33"/>
+    <mergeCell ref="Q30:Q33"/>
+    <mergeCell ref="R30:R33"/>
+    <mergeCell ref="S30:S33"/>
+    <mergeCell ref="T30:T33"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="H47:I48"/>
+    <mergeCell ref="K35:Q36"/>
+    <mergeCell ref="K37:Q74"/>
+    <mergeCell ref="R35:X35"/>
+    <mergeCell ref="R36:R40"/>
+    <mergeCell ref="X36:X40"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="H37:I38"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="G35:I36"/>
+    <mergeCell ref="H41:I42"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="H43:I44"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="H45:I46"/>
+    <mergeCell ref="H39:I40"/>
+    <mergeCell ref="G41:G42"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC7FB991-26FD-4149-AB03-88A0259D5578}">
+  <dimension ref="A2:XFD1048575"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="72.28515625" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" customWidth="1"/>
+    <col min="11" max="11" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="G2" s="118"/>
+      <c r="H2" s="118"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+    </row>
+    <row r="3" spans="1:12" ht="47.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="120" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" s="120"/>
+      <c r="C3" s="60" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" s="60" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" s="60" t="s">
+        <v>119</v>
+      </c>
+      <c r="F3" s="58"/>
+      <c r="G3" s="119" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="119"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="61" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="121" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" s="71" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" s="124">
+        <v>90</v>
+      </c>
+      <c r="D4" s="129">
+        <v>4000</v>
+      </c>
+      <c r="E4" s="123">
+        <v>10000</v>
+      </c>
+      <c r="F4" s="58"/>
+      <c r="G4" s="56" t="s">
+        <v>123</v>
+      </c>
+      <c r="H4" s="133">
+        <v>10</v>
+      </c>
+      <c r="I4" s="58"/>
+      <c r="J4" s="60" t="s">
+        <v>129</v>
+      </c>
+      <c r="K4" s="62">
+        <f>H4*C4+H5*C5+H6*C6+H7*C7+H8*C8+H9*C9</f>
+        <v>2160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="117"/>
+      <c r="B5" s="65" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" s="132">
+        <v>55</v>
+      </c>
+      <c r="D5" s="126">
+        <v>1500</v>
+      </c>
+      <c r="E5" s="122"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="56" t="s">
+        <v>125</v>
+      </c>
+      <c r="H5" s="131">
+        <v>5</v>
+      </c>
+      <c r="I5" s="58"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="58"/>
+    </row>
+    <row r="6" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="116" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" s="64" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" s="130">
+        <v>25</v>
+      </c>
+      <c r="D6" s="129">
+        <v>2000</v>
+      </c>
+      <c r="E6" s="123">
+        <v>3000</v>
+      </c>
+      <c r="F6" s="58"/>
+      <c r="G6" s="69" t="s">
+        <v>124</v>
+      </c>
+      <c r="H6" s="128">
+        <v>15</v>
+      </c>
+      <c r="I6" s="58"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="58"/>
+    </row>
+    <row r="7" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="117"/>
+      <c r="B7" s="72" t="s">
+        <v>132</v>
+      </c>
+      <c r="C7" s="127">
+        <v>20</v>
+      </c>
+      <c r="D7" s="126">
+        <v>1200</v>
+      </c>
+      <c r="E7" s="122"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="56" t="s">
+        <v>126</v>
+      </c>
+      <c r="H7" s="70">
+        <v>18</v>
+      </c>
+      <c r="I7" s="58"/>
+      <c r="J7" s="58"/>
+      <c r="K7" s="58"/>
+    </row>
+    <row r="8" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="116" t="s">
+        <v>122</v>
+      </c>
+      <c r="B8" s="64" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8" s="125">
+        <v>10</v>
+      </c>
+      <c r="D8" s="124">
+        <v>1000</v>
+      </c>
+      <c r="E8" s="123">
+        <v>1000</v>
+      </c>
+      <c r="F8" s="58"/>
+      <c r="G8" s="69" t="s">
+        <v>127</v>
+      </c>
+      <c r="H8" s="68">
+        <v>20</v>
+      </c>
+      <c r="I8" s="58"/>
+      <c r="J8" s="58"/>
+      <c r="K8" s="58"/>
+    </row>
+    <row r="9" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="117"/>
+      <c r="B9" s="72" t="s">
+        <v>135</v>
+      </c>
+      <c r="C9" s="66">
+        <v>5</v>
+      </c>
+      <c r="D9" s="67">
+        <v>800</v>
+      </c>
+      <c r="E9" s="122"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="57" t="s">
+        <v>128</v>
+      </c>
+      <c r="H9" s="63">
+        <v>10</v>
+      </c>
+      <c r="I9" s="58"/>
+      <c r="J9" s="58"/>
+      <c r="K9" s="58"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B11" s="184"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="79" t="s">
+        <v>174</v>
+      </c>
+      <c r="B12" s="184">
+        <v>279000</v>
+      </c>
+      <c r="G12" s="186" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="79" t="s">
+        <v>207</v>
+      </c>
+      <c r="B13" s="184">
+        <v>99000</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" s="79" t="s">
+        <v>175</v>
+      </c>
+      <c r="H13">
+        <f>SUM(H4:H5)*2</f>
+        <v>30</v>
+      </c>
+      <c r="I13" s="79" t="s">
+        <v>211</v>
+      </c>
+      <c r="J13">
+        <f>SUM(H6:H7)</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="79" t="s">
+        <v>208</v>
+      </c>
+      <c r="B14" s="185">
+        <v>20</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14" s="79" t="s">
+        <v>156</v>
+      </c>
+      <c r="H14">
+        <f>SUM(H4:H5)</f>
+        <v>15</v>
+      </c>
+      <c r="I14" s="79" t="s">
+        <v>211</v>
+      </c>
+      <c r="J14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="79" t="s">
+        <v>209</v>
+      </c>
+      <c r="B15" s="184">
+        <v>30000</v>
+      </c>
+      <c r="F15">
+        <v>3</v>
+      </c>
+      <c r="G15" s="79" t="s">
+        <v>157</v>
+      </c>
+      <c r="H15" s="187">
+        <f>H4*E4+H5*E4</f>
+        <v>150000</v>
+      </c>
+      <c r="I15" s="79" t="s">
+        <v>215</v>
+      </c>
+      <c r="J15" s="184">
+        <f>B16</f>
+        <v>140000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="79" t="s">
+        <v>216</v>
+      </c>
+      <c r="B16" s="184">
+        <v>140000</v>
+      </c>
+      <c r="F16">
+        <v>4</v>
+      </c>
+      <c r="G16" t="s">
+        <v>158</v>
+      </c>
+      <c r="H16" s="187">
+        <f>H6*E6+H7*E6</f>
+        <v>99000</v>
+      </c>
+      <c r="I16" s="79" t="s">
+        <v>211</v>
+      </c>
+      <c r="J16" s="184">
+        <f>B13</f>
+        <v>99000</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B17" s="184"/>
+      <c r="F17">
+        <v>5</v>
+      </c>
+      <c r="G17" t="s">
+        <v>159</v>
+      </c>
+      <c r="H17" s="187">
+        <f>H8*E8+H9*E8</f>
+        <v>30000</v>
+      </c>
+      <c r="I17" s="79" t="s">
+        <v>215</v>
+      </c>
+      <c r="J17" s="184">
+        <f>B15</f>
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B18" s="184"/>
+      <c r="F18">
+        <v>6</v>
+      </c>
+      <c r="G18" t="s">
+        <v>161</v>
+      </c>
+      <c r="H18" s="187">
+        <f>H4*E4+H5*E4+H6*E6+H7*E6+H8*E8+H9*E8</f>
+        <v>279000</v>
+      </c>
+      <c r="I18" s="79" t="s">
+        <v>211</v>
+      </c>
+      <c r="J18" s="184">
+        <f>B12</f>
+        <v>279000</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B19" s="184"/>
+      <c r="F19">
+        <v>7</v>
+      </c>
+      <c r="G19" t="s">
+        <v>163</v>
+      </c>
+      <c r="H19">
+        <f>H4*D4+H5*D5+H6*D6+H7*D7+H8*D8+H9*D9</f>
+        <v>127100</v>
+      </c>
+      <c r="I19" s="79" t="s">
+        <v>215</v>
+      </c>
+      <c r="J19">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="184"/>
+      <c r="F20" s="185">
+        <v>8</v>
+      </c>
+      <c r="G20" s="79" t="s">
+        <v>212</v>
+      </c>
+      <c r="H20">
+        <f>H4</f>
+        <v>10</v>
+      </c>
+      <c r="I20" s="79" t="s">
+        <v>211</v>
+      </c>
+      <c r="J20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="184"/>
+      <c r="F21" s="185">
+        <v>9</v>
+      </c>
+      <c r="G21" s="79" t="s">
+        <v>213</v>
+      </c>
+      <c r="H21">
+        <f>H6</f>
+        <v>15</v>
+      </c>
+      <c r="I21" s="79" t="s">
+        <v>211</v>
+      </c>
+      <c r="J21">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="184"/>
+      <c r="F22" s="185">
+        <v>10</v>
+      </c>
+      <c r="G22" s="79" t="s">
+        <v>214</v>
+      </c>
+      <c r="H22">
+        <f>H8</f>
+        <v>20</v>
+      </c>
+      <c r="I22" s="79" t="s">
+        <v>211</v>
+      </c>
+      <c r="J22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="183"/>
+      <c r="F23" s="185">
+        <v>11</v>
+      </c>
+      <c r="G23" s="79" t="s">
+        <v>217</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="183"/>
+      <c r="F24" s="185"/>
+      <c r="G24" s="79"/>
+    </row>
+    <row r="25" spans="2:10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F25" s="185"/>
+    </row>
+    <row r="26" spans="2:10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F26" s="185"/>
+    </row>
+    <row r="27" spans="2:10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F27" s="185"/>
+    </row>
+    <row r="28" spans="2:10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F28" s="185"/>
+    </row>
+    <row r="29" spans="2:10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F29" s="185"/>
+    </row>
+    <row r="30" spans="2:10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F30" s="185"/>
+    </row>
+    <row r="31" spans="2:10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F31" s="185"/>
+    </row>
+    <row r="32" spans="2:10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F32" s="185"/>
+    </row>
+    <row r="36" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="1048549" spans="16384:16384" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="XFD1048549">
+        <f>solver_pre</f>
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="1048550" spans="16384:16384" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="XFD1048550">
+        <f>solver_scl</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1048551" spans="16384:16384" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="XFD1048551">
+        <f>solver_rlx</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1048552" spans="16384:16384" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="XFD1048552">
+        <f>solver_tol</f>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="1048553" spans="16384:16384" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="XFD1048553">
+        <f>solver_cvg</f>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="1048554" spans="16384:16384" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="XFD1048554" t="e" cm="1">
+        <f t="array" ref="XFD1048554">AREAS(solver_adj1)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="1048555" spans="16384:16384" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="XFD1048555">
+        <f>solver_ssz</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="1048556" spans="16384:16384" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="XFD1048556">
+        <f>solver_rsd</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1048557" spans="16384:16384" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="XFD1048557">
+        <f>solver_mrt</f>
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="1048558" spans="16384:16384" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="XFD1048558">
+        <f>solver_mni</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="1048559" spans="16384:16384" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="XFD1048559">
+        <f>solver_rbv</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1048560" spans="16384:16384" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="XFD1048560">
+        <f>solver_neg</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1048561" spans="16384:16384" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="XFD1048561" t="e" cm="1">
+        <f t="array" ref="XFD1048561">solver_ntr</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="1048562" spans="16384:16384" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="XFD1048562" t="e" cm="1">
+        <f t="array" ref="XFD1048562">solver_acc</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="1048563" spans="16384:16384" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="XFD1048563" t="e" cm="1">
+        <f t="array" ref="XFD1048563">solver_res</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="1048564" spans="16384:16384" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="XFD1048564" t="e" cm="1">
+        <f t="array" ref="XFD1048564">solver_ars</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="1048565" spans="16384:16384" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="XFD1048565" t="e" cm="1">
+        <f t="array" ref="XFD1048565">solver_sta</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="1048566" spans="16384:16384" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="XFD1048566" t="e" cm="1">
+        <f t="array" ref="XFD1048566">solver_met</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="1048567" spans="16384:16384" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="XFD1048567" t="e" cm="1">
+        <f t="array" ref="XFD1048567">solver_soc</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="1048568" spans="16384:16384" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="XFD1048568" t="e" cm="1">
+        <f t="array" ref="XFD1048568">solver_lpt</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="1048569" spans="16384:16384" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="XFD1048569" t="e" cm="1">
+        <f t="array" ref="XFD1048569">solver_lpp</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="1048570" spans="16384:16384" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="XFD1048570" t="e" cm="1">
+        <f t="array" ref="XFD1048570">solver_gap</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="1048571" spans="16384:16384" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="XFD1048571" t="e" cm="1">
+        <f t="array" ref="XFD1048571">solver_ips</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="1048572" spans="16384:16384" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="XFD1048572" t="e" cm="1">
+        <f t="array" ref="XFD1048572">solver_fea</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="1048573" spans="16384:16384" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="XFD1048573" t="e" cm="1">
+        <f t="array" ref="XFD1048573">solver_ipi</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="1048574" spans="16384:16384" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="XFD1048574" t="e" cm="1">
+        <f t="array" ref="XFD1048574">solver_ipd</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="1048575" spans="16384:16384" customFormat="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <mergeCells count="9">
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="E6:E7"/>
@@ -10448,17 +13400,5 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{F7C9EE02-42E1-4005-9D12-6889AFFD525C}">
-      <x15:webExtensions xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x15:webExtension appRef="{83B5D8B2-AF49-6D41-B7BB-A01E4097B078}">
-          <xm:f>'Q4.Flamingo Grill'!1:1048576</xm:f>
-        </x15:webExtension>
-        <x15:webExtension appRef="{A0C87E43-B8AD-0641-A98E-254343A9F0BF}">
-          <xm:f>'Q4.Flamingo Grill'!XFD1048550:XFD1048575</xm:f>
-        </x15:webExtension>
-      </x15:webExtensions>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>